<commit_message>
almost finished the testing on dense matrix
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>numPipes</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>numCols</t>
+  </si>
+  <si>
+    <t>dataSize</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>Dense matrix for the same design</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>nil</t>
   </si>
 </sst>
 </file>
@@ -78,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,18 +107,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,62 +450,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="H2" s="2"/>
+      <c r="N2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="N3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -479,10 +557,32 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="N4" s="7">
+        <v>8192</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+      <c r="P4" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>663552</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.165078</v>
+      </c>
+      <c r="S4" s="8">
+        <v>1.2115000000000001E-2</v>
+      </c>
+      <c r="T4" s="8">
+        <f>S4/S4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -501,10 +601,28 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>6709248</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0.152341</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1.3128000000000001E-2</v>
+      </c>
+      <c r="T5" s="8">
+        <f t="shared" ref="T5:T6" si="0">S5/S5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -523,10 +641,28 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>67108864</v>
+      </c>
+      <c r="R6" s="8">
+        <v>0.15112</v>
+      </c>
+      <c r="S6" s="8">
+        <v>1.3233999999999999E-2</v>
+      </c>
+      <c r="T6" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -545,13 +681,197 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7">
+        <v>2</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>663552</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>6709248</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="T8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>67108864</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="T9" s="8"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N10" s="7"/>
+      <c r="O10" s="7">
+        <v>4</v>
+      </c>
+      <c r="P10" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>663552</v>
+      </c>
+      <c r="R10" s="8">
+        <v>8.8065000000000004E-2</v>
+      </c>
+      <c r="S10" s="8">
+        <v>2.2710000000000001E-2</v>
+      </c>
+      <c r="T10" s="8">
+        <f>S10/S4</f>
+        <v>1.8745356995460174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>6709248</v>
+      </c>
+      <c r="R11" s="8">
+        <v>4.3457000000000003E-2</v>
+      </c>
+      <c r="S11" s="8">
+        <v>4.6023000000000001E-2</v>
+      </c>
+      <c r="T11" s="8">
+        <f>S11/S5</f>
+        <v>3.5057129798903106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>67108864</v>
+      </c>
+      <c r="R12" s="8">
+        <v>3.9405000000000003E-2</v>
+      </c>
+      <c r="S12" s="8">
+        <v>5.0755000000000002E-2</v>
+      </c>
+      <c r="T12" s="8">
+        <f>S12/S6</f>
+        <v>3.8351972192836636</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N13" s="7"/>
+      <c r="O13" s="7">
+        <v>8</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>663552</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0.121377</v>
+      </c>
+      <c r="S13" s="8">
+        <v>1.6478E-2</v>
+      </c>
+      <c r="T13" s="8">
+        <f>S13/S4</f>
+        <v>1.3601320676846882</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>6709248</v>
+      </c>
+      <c r="R14" s="8">
+        <v>2.9537999999999998E-2</v>
+      </c>
+      <c r="S14" s="8">
+        <v>6.7710000000000006E-2</v>
+      </c>
+      <c r="T14" s="8">
+        <f>S14/S5</f>
+        <v>5.157678244972578</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>67108864</v>
+      </c>
+      <c r="R15" s="8">
+        <v>2.0851999999999999E-2</v>
+      </c>
+      <c r="S15" s="8">
+        <v>9.5916000000000001E-2</v>
+      </c>
+      <c r="T15" s="8">
+        <f>S15/S6</f>
+        <v>7.2476953302100657</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="10">
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="A4:A7"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="N4:N15"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="O13:O15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated with numPipes = 2 data.
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>numPipes</t>
   </si>
@@ -65,16 +65,13 @@
   </si>
   <si>
     <t>Ratio</t>
-  </si>
-  <si>
-    <t>nil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +83,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,24 +130,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -453,7 +460,7 @@
   <dimension ref="A2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,24 +473,24 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="N2" s="5" t="s">
+      <c r="H2" s="5"/>
+      <c r="N2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="4"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -510,33 +517,33 @@
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="6">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -557,32 +564,32 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="8">
         <v>8192</v>
       </c>
-      <c r="O4" s="7">
-        <v>1</v>
-      </c>
-      <c r="P4" s="8">
+      <c r="O4" s="8">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
         <v>0.01</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="4">
         <v>663552</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4" s="4">
         <v>0.165078</v>
       </c>
-      <c r="S4" s="8">
+      <c r="S4" s="4">
         <v>1.2115000000000001E-2</v>
       </c>
-      <c r="T4" s="8">
+      <c r="T4" s="4">
         <f>S4/S4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -601,28 +608,28 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8">
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="4">
         <v>0.1</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="4">
         <v>6709248</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="4">
         <v>0.152341</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5" s="4">
         <v>1.3128000000000001E-2</v>
       </c>
-      <c r="T5" s="8">
+      <c r="T5" s="4">
         <f t="shared" ref="T5:T6" si="0">S5/S5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -641,28 +648,28 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="8">
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4">
         <v>67108864</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="4">
         <v>0.15112</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="4">
         <v>1.3233999999999999E-2</v>
       </c>
-      <c r="T6" s="8">
+      <c r="T6" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -681,184 +688,193 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7">
+      <c r="N7" s="8"/>
+      <c r="O7" s="8">
         <v>2</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="4">
         <v>0.01</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q7" s="4">
         <v>663552</v>
       </c>
-      <c r="R7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="T7" s="8"/>
+      <c r="R7" s="4">
+        <v>0.100855</v>
+      </c>
+      <c r="S7" s="4">
+        <v>1.9831000000000001E-2</v>
+      </c>
+      <c r="T7" s="4">
+        <f>S7/S4</f>
+        <v>1.6368964094098226</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="8">
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="4">
         <v>0.1</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8" s="4">
         <v>6709248</v>
       </c>
-      <c r="R8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="T8" s="8"/>
+      <c r="R8" s="4">
+        <v>7.8479999999999994E-2</v>
+      </c>
+      <c r="S8" s="4">
+        <v>2.5484E-2</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" ref="T8:T9" si="1">S8/S5</f>
+        <v>1.9411943936624008</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="8">
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="4">
         <v>67108864</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="T9" s="8"/>
+      <c r="R9" s="4">
+        <v>7.6520000000000005E-2</v>
+      </c>
+      <c r="S9" s="4">
+        <v>2.6137000000000001E-2</v>
+      </c>
+      <c r="T9" s="9">
+        <f t="shared" si="1"/>
+        <v>1.9749886655584104</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="7"/>
-      <c r="O10" s="7">
+      <c r="N10" s="8"/>
+      <c r="O10" s="8">
         <v>4</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="4">
         <v>0.01</v>
       </c>
-      <c r="Q10" s="8">
+      <c r="Q10" s="4">
         <v>663552</v>
       </c>
-      <c r="R10" s="8">
+      <c r="R10" s="4">
         <v>8.8065000000000004E-2</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10" s="4">
         <v>2.2710000000000001E-2</v>
       </c>
-      <c r="T10" s="8">
+      <c r="T10" s="4">
         <f>S10/S4</f>
         <v>1.8745356995460174</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="8">
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="4">
         <v>0.1</v>
       </c>
-      <c r="Q11" s="8">
+      <c r="Q11" s="4">
         <v>6709248</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11" s="4">
         <v>4.3457000000000003E-2</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11" s="4">
         <v>4.6023000000000001E-2</v>
       </c>
-      <c r="T11" s="8">
+      <c r="T11" s="4">
         <f>S11/S5</f>
         <v>3.5057129798903106</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="8">
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4">
         <v>67108864</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12" s="4">
         <v>3.9405000000000003E-2</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12" s="4">
         <v>5.0755000000000002E-2</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" s="9">
         <f>S12/S6</f>
         <v>3.8351972192836636</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N13" s="7"/>
-      <c r="O13" s="7">
+      <c r="N13" s="8"/>
+      <c r="O13" s="8">
         <v>8</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="4">
         <v>0.01</v>
       </c>
-      <c r="Q13" s="8">
+      <c r="Q13" s="4">
         <v>663552</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13" s="4">
         <v>0.121377</v>
       </c>
-      <c r="S13" s="8">
+      <c r="S13" s="4">
         <v>1.6478E-2</v>
       </c>
-      <c r="T13" s="8">
+      <c r="T13" s="4">
         <f>S13/S4</f>
         <v>1.3601320676846882</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="8">
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="4">
         <v>0.1</v>
       </c>
-      <c r="Q14" s="8">
+      <c r="Q14" s="4">
         <v>6709248</v>
       </c>
-      <c r="R14" s="8">
+      <c r="R14" s="4">
         <v>2.9537999999999998E-2</v>
       </c>
-      <c r="S14" s="8">
+      <c r="S14" s="4">
         <v>6.7710000000000006E-2</v>
       </c>
-      <c r="T14" s="8">
+      <c r="T14" s="4">
         <f>S14/S5</f>
         <v>5.157678244972578</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="8">
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
         <v>67108864</v>
       </c>
-      <c r="R15" s="8">
+      <c r="R15" s="4">
         <v>2.0851999999999999E-2</v>
       </c>
-      <c r="S15" s="8">
+      <c r="S15" s="4">
         <v>9.5916000000000001E-2</v>
       </c>
-      <c r="T15" s="8">
+      <c r="T15" s="9">
         <f>S15/S6</f>
         <v>7.2476953302100657</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I26" s="4"/>
+      <c r="I26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
add Standard CSRp first data
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
+    <sheet name="Standard CSRp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>numPipes</t>
   </si>
@@ -65,13 +66,25 @@
   </si>
   <si>
     <t>Ratio</t>
+  </si>
+  <si>
+    <t>speed test</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>BRAM</t>
+  </si>
+  <si>
+    <t>Dense matrix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +103,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -138,6 +157,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -150,8 +175,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,23 +516,23 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="N2" s="7" t="s">
+      <c r="H2" s="7"/>
+      <c r="N2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -540,10 +583,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -564,10 +607,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="10">
         <v>8192</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="10">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -588,8 +631,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -608,8 +651,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -628,8 +671,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -648,8 +691,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -662,14 +705,14 @@
       <c r="S6" s="4">
         <v>1.3233999999999999E-2</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -688,8 +731,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8">
+      <c r="N7" s="10"/>
+      <c r="O7" s="10">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -710,8 +753,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -730,8 +773,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -744,14 +787,14 @@
       <c r="S9" s="4">
         <v>2.6137000000000001E-2</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="6">
         <f t="shared" si="1"/>
         <v>1.9749886655584104</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="8"/>
-      <c r="O10" s="8">
+      <c r="N10" s="10"/>
+      <c r="O10" s="10">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -772,8 +815,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -792,8 +835,8 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -806,14 +849,14 @@
       <c r="S12" s="4">
         <v>5.0755000000000002E-2</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="6">
         <f>S12/S6</f>
         <v>3.8351972192836636</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N13" s="8"/>
-      <c r="O13" s="8">
+      <c r="N13" s="10"/>
+      <c r="O13" s="10">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -834,8 +877,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -854,8 +897,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -868,7 +911,7 @@
       <c r="S15" s="4">
         <v>9.5916000000000001E-2</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="6">
         <f>S15/S6</f>
         <v>7.2476953302100657</v>
       </c>
@@ -892,4 +935,220 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>8192</v>
+      </c>
+      <c r="B6" s="10">
+        <v>67108864</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="13">
+        <v>4</v>
+      </c>
+      <c r="D8" s="17">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E8" s="17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F8" s="17">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>3.9098000000000001E-2</v>
+      </c>
+      <c r="H8" s="14">
+        <v>5.1152999999999997E-2</v>
+      </c>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="13">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="16">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="16">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="16">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="16">
+        <v>128</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="16">
+        <v>256</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add few more data
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Coding/Research/ImperialSummerReports/assets/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17540" activeTab="1"/>
+    <workbookView xWindow="1020" yWindow="465" windowWidth="27780" windowHeight="17535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
     <sheet name="Standard CSRp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>numPipes</t>
   </si>
@@ -88,6 +83,9 @@
   </si>
   <si>
     <t>Dense matrix</t>
+  </si>
+  <si>
+    <t>Time (us)</t>
   </si>
 </sst>
 </file>
@@ -159,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -185,6 +183,18 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -199,15 +209,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,36 +520,36 @@
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="N2" s="13" t="s">
+      <c r="H2" s="15"/>
+      <c r="N2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -595,11 +596,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="16">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -620,10 +621,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="18">
         <v>8192</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="18">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -643,9 +644,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -664,8 +665,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -683,9 +684,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -704,8 +705,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -723,9 +724,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -744,8 +745,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14">
+      <c r="N7" s="18"/>
+      <c r="O7" s="18">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -765,9 +766,9 @@
         <v>1.6368964094098226</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -785,9 +786,9 @@
         <v>1.9411943936624008</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -805,9 +806,9 @@
         <v>1.9749886655584104</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N10" s="14"/>
-      <c r="O10" s="14">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N10" s="18"/>
+      <c r="O10" s="18">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -827,9 +828,9 @@
         <v>1.8745356995460174</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -847,9 +848,9 @@
         <v>3.5057129798903106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -867,9 +868,9 @@
         <v>3.8351972192836636</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N13" s="14"/>
-      <c r="O13" s="14">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N13" s="18"/>
+      <c r="O13" s="18">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -889,9 +890,9 @@
         <v>1.3601320676846882</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -909,9 +910,9 @@
         <v>5.157678244972578</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -929,7 +930,7 @@
         <v>7.2476953302100657</v>
       </c>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="2"/>
     </row>
   </sheetData>
@@ -954,53 +955,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="17"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="15"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>7</v>
@@ -1020,11 +1021,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="14">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
         <v>8192</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="18">
         <v>67108864</v>
       </c>
       <c r="C6" s="8">
@@ -1045,13 +1046,13 @@
       <c r="H6" s="6">
         <v>1.3198E-2</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="8">
         <v>2</v>
       </c>
@@ -1066,11 +1067,11 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="8">
         <v>4</v>
       </c>
@@ -1089,14 +1090,14 @@
       <c r="H8" s="6">
         <v>5.1152999999999997E-2</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="12">
         <f>H8/H6</f>
         <v>3.8758145173511136</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="8">
         <v>8</v>
       </c>
@@ -1109,13 +1110,20 @@
       <c r="F9" s="10">
         <v>8.1799999999999998E-2</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="G9" s="11">
+        <v>1.9286999999999999E-2</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.103695</v>
+      </c>
+      <c r="I9" s="12">
+        <f>H9/H6</f>
+        <v>7.8568722533717228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="9">
         <v>16</v>
       </c>
@@ -1128,13 +1136,20 @@
       <c r="F10" s="10">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+      <c r="G10" s="11">
+        <v>1.0292000000000001E-2</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.194331</v>
+      </c>
+      <c r="I10" s="12">
+        <f>H10/H6</f>
+        <v>14.724276405515988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="9">
         <v>32</v>
       </c>
@@ -1147,13 +1162,20 @@
       <c r="F11" s="10">
         <v>0.28050000000000003</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="G11" s="11">
+        <v>5.7780000000000001E-3</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0.34616200000000003</v>
+      </c>
+      <c r="I11" s="6">
+        <f>H11/H6</f>
+        <v>26.228367934535537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="9">
         <v>64</v>
       </c>
@@ -1177,38 +1199,38 @@
         <v>29.68252765570541</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="9">
         <v>128</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="13">
         <v>0.45450000000000002</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="13">
         <v>0.127</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="13">
         <v>0.99719999999999998</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="9">
         <v>256</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="13">
         <v>0.87560000000000004</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="13">
         <v>0.254</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="13">
         <v>1.9812000000000001</v>
       </c>
       <c r="G14" s="6"/>

</xml_diff>

<commit_message>
updated dual ports ROM
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Coding/Research/ImperialSummerReports/assets/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="465" windowWidth="27780" windowHeight="17535" activeTab="1"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
     <sheet name="Standard CSRp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>numPipes</t>
   </si>
@@ -101,6 +106,9 @@
   </si>
   <si>
     <t>freq(MHz)</t>
+  </si>
+  <si>
+    <t>Timing failed</t>
   </si>
 </sst>
 </file>
@@ -210,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -242,6 +250,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -257,7 +278,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,16 +287,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -589,36 +606,36 @@
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="N2" s="15" t="s">
+      <c r="H2" s="18"/>
+      <c r="N2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -665,11 +682,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="19">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -690,10 +707,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="21">
         <v>8192</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="21">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -713,9 +730,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -734,8 +751,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -753,9 +770,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -774,8 +791,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -793,9 +810,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -814,8 +831,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16">
+      <c r="N7" s="21"/>
+      <c r="O7" s="21">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -835,9 +852,9 @@
         <v>1.6368964094098226</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -855,9 +872,9 @@
         <v>1.9411943936624008</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -875,9 +892,9 @@
         <v>1.9749886655584104</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="16"/>
-      <c r="O10" s="16">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N10" s="21"/>
+      <c r="O10" s="21">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -897,9 +914,9 @@
         <v>1.8745356995460174</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -917,9 +934,9 @@
         <v>3.5057129798903106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -937,9 +954,9 @@
         <v>3.8351972192836636</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N13" s="16"/>
-      <c r="O13" s="16">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N13" s="21"/>
+      <c r="O13" s="21">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -959,9 +976,9 @@
         <v>1.3601320676846882</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -979,9 +996,9 @@
         <v>5.157678244972578</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -999,7 +1016,7 @@
         <v>7.2476953302100657</v>
       </c>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I26" s="2"/>
     </row>
   </sheetData>
@@ -1024,86 +1041,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="184" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="19" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="19" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="19" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="21"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="25"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="2"/>
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="15"/>
+      <c r="M4" s="20"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="15"/>
+      <c r="Q4" s="20"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1153,8 +1170,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
         <v>8192</v>
       </c>
       <c r="B6" s="6">
@@ -1169,7 +1186,7 @@
       <c r="E6" s="8">
         <v>2.2599999999999999E-2</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="15">
         <v>200</v>
       </c>
       <c r="G6" s="8">
@@ -1181,7 +1198,7 @@
       <c r="I6" s="11">
         <v>2.6120000000000001E-2</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="16">
         <v>1</v>
       </c>
       <c r="K6" s="8">
@@ -1193,7 +1210,7 @@
       <c r="M6" s="11">
         <v>2.6098E-2</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="16">
         <v>1</v>
       </c>
       <c r="O6" s="8">
@@ -1205,12 +1222,12 @@
       <c r="Q6" s="11">
         <v>2.6086999999999999E-2</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -1223,7 +1240,7 @@
       <c r="E7" s="8">
         <v>3.1E-2</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="15">
         <v>200</v>
       </c>
       <c r="G7" s="8">
@@ -1235,7 +1252,7 @@
       <c r="I7" s="11">
         <v>5.1270999999999997E-2</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="16">
         <f>I7/I6</f>
         <v>1.9629019908116385</v>
       </c>
@@ -1248,7 +1265,7 @@
       <c r="M7" s="11">
         <v>5.1462000000000001E-2</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="16">
         <f>M7/M6</f>
         <v>1.9718752394819528</v>
       </c>
@@ -1261,13 +1278,13 @@
       <c r="Q7" s="11">
         <v>5.1159000000000003E-2</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="16">
         <f>Q7/Q6</f>
         <v>1.961091731513781</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -1280,7 +1297,7 @@
       <c r="E8" s="8">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="15">
         <v>200</v>
       </c>
       <c r="G8" s="8">
@@ -1292,7 +1309,7 @@
       <c r="I8" s="11">
         <v>9.8136000000000001E-2</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="16">
         <f>I8/I6</f>
         <v>3.7571209800918837</v>
       </c>
@@ -1305,7 +1322,7 @@
       <c r="M8" s="11">
         <v>9.8801E-2</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="16">
         <f>M8/M6</f>
         <v>3.7857690244463176</v>
       </c>
@@ -1318,13 +1335,13 @@
       <c r="Q8" s="11">
         <v>9.7436999999999996E-2</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="16">
         <f>Q8/Q6</f>
         <v>3.7350787748687084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -1337,7 +1354,7 @@
       <c r="E9" s="8">
         <v>8.1799999999999998E-2</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="15">
         <v>200</v>
       </c>
       <c r="G9" s="8">
@@ -1349,7 +1366,7 @@
       <c r="I9" s="11">
         <v>0.174731</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="16">
         <f>I9/I6</f>
         <v>6.6895482388973964</v>
       </c>
@@ -1362,7 +1379,7 @@
       <c r="M9" s="11">
         <v>0.16947699999999999</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="16">
         <f>M9/M6</f>
         <v>6.4938692620124145</v>
       </c>
@@ -1375,13 +1392,13 @@
       <c r="Q9" s="11">
         <v>0.16950999999999999</v>
       </c>
-      <c r="R9" s="24">
+      <c r="R9" s="16">
         <f>Q9/Q6</f>
         <v>6.4978725035458273</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
       <c r="B10" s="7">
         <v>16</v>
       </c>
@@ -1394,7 +1411,7 @@
       <c r="E10" s="8">
         <v>0.14799999999999999</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="15">
         <v>200</v>
       </c>
       <c r="G10" s="8">
@@ -1406,7 +1423,7 @@
       <c r="I10" s="11">
         <v>0.28039199999999997</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="16">
         <f>I10/I6</f>
         <v>10.734762633996937</v>
       </c>
@@ -1419,7 +1436,7 @@
       <c r="M10" s="11">
         <v>0.22001200000000001</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="16">
         <f>M10/M6</f>
         <v>8.4302245382787966</v>
       </c>
@@ -1432,13 +1449,13 @@
       <c r="Q10" s="11">
         <v>0.25703799999999999</v>
       </c>
-      <c r="R10" s="24">
+      <c r="R10" s="16">
         <f>Q10/Q6</f>
         <v>9.8531069114884815</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
       <c r="B11" s="7">
         <v>32</v>
       </c>
@@ -1451,7 +1468,7 @@
       <c r="E11" s="8">
         <v>0.28050000000000003</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="15">
         <v>200</v>
       </c>
       <c r="G11" s="8">
@@ -1463,7 +1480,7 @@
       <c r="I11" s="11">
         <v>0.229377</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="17">
         <f>I11/I6</f>
         <v>8.7816615620214389</v>
       </c>
@@ -1476,7 +1493,7 @@
       <c r="M11" s="11">
         <v>0.15629299999999999</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="17">
         <f>M11/M6</f>
         <v>5.9886964518353896</v>
       </c>
@@ -1489,13 +1506,13 @@
       <c r="Q11" s="11">
         <v>0.21099599999999999</v>
       </c>
-      <c r="R11" s="25">
+      <c r="R11" s="17">
         <f>Q11/Q6</f>
         <v>8.088166519722467</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
       <c r="B12" s="7">
         <v>64</v>
       </c>
@@ -1508,47 +1525,24 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="23">
-        <v>200</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
-        <v>5.1050000000000002E-3</v>
-      </c>
-      <c r="I12" s="11">
-        <v>0.39174999999999999</v>
-      </c>
-      <c r="J12" s="25">
-        <f>I12/I6</f>
-        <v>14.998085758039815</v>
-      </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="11">
-        <v>5.1050000000000002E-3</v>
-      </c>
-      <c r="M12" s="11">
-        <v>0.39174999999999999</v>
-      </c>
-      <c r="N12" s="25">
-        <f>M12/M6</f>
-        <v>15.010728791478273</v>
-      </c>
-      <c r="O12" s="8"/>
-      <c r="P12" s="11">
-        <v>5.1050000000000002E-3</v>
-      </c>
-      <c r="Q12" s="11">
-        <v>0.39174999999999999</v>
-      </c>
-      <c r="R12" s="25">
-        <f>Q12/Q6</f>
-        <v>15.017058304902825</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="F12" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="28"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
       <c r="B13" s="7">
         <v>128</v>
       </c>
@@ -1575,8 +1569,8 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
       <c r="B14" s="7">
         <v>256</v>
       </c>
@@ -1604,18 +1598,19 @@
       <c r="R14" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F12:R12"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C4:E4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:R3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated with BCSR format's result
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="1"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
     <sheet name="Standard CSRp" sheetId="2" r:id="rId2"/>
+    <sheet name="BCSR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>numPipes</t>
   </si>
@@ -109,13 +110,91 @@
   </si>
   <si>
     <t>Timing failed</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>ROM size</t>
+  </si>
+  <si>
+    <t>Stream
+Frequency</t>
+  </si>
+  <si>
+    <t>Resource Usage</t>
+  </si>
+  <si>
+    <t>Multipliers</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Estimated
+Time(s)</t>
+  </si>
+  <si>
+    <t>Total
+Time(s)</t>
+  </si>
+  <si>
+    <t>Time per
+element(us)</t>
+  </si>
+  <si>
+    <t>Bandwidth
+(MHz)</t>
+  </si>
+  <si>
+    <t>Estimated
+Bandwidth(MHz)</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Dense Matrix: Special study on 4 X 16 block with 8192 ROM size</t>
+  </si>
+  <si>
+    <t>nnz</t>
+  </si>
+  <si>
+    <t>Esti. Time</t>
+  </si>
+  <si>
+    <t>Esti. Band</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Real/Esti.</t>
+  </si>
+  <si>
+    <t>Comp to 1.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +224,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,7 +260,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -214,11 +320,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -275,6 +422,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -287,17 +443,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -311,6 +515,1100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1080" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" charset="0"/>
+                <a:ea typeface="Consolas" charset="0"/>
+                <a:cs typeface="Consolas" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Bandwidth for different</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> m value</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1080" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" charset="0"/>
+              <a:ea typeface="Consolas" charset="0"/>
+              <a:cs typeface="Consolas" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Bandwidth</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" charset="0"/>
+                    <a:ea typeface="Consolas" charset="0"/>
+                    <a:cs typeface="Consolas" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>BCSR!$B$25:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8192.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24576.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32768.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40960.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49152.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57344.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65536.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BCSR!$H$25:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>146.75565</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184.423023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>201.652462</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>211.523561</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>221.648331</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>229.297049</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>236.224314</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>244.053754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="b"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2096734560"/>
+        <c:axId val="-2091307792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2096734560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" charset="0"/>
+                    <a:ea typeface="Consolas" charset="0"/>
+                    <a:cs typeface="Consolas" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> value</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Consolas" charset="0"/>
+                  <a:ea typeface="Consolas" charset="0"/>
+                  <a:cs typeface="Consolas" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" charset="0"/>
+                <a:ea typeface="Consolas" charset="0"/>
+                <a:cs typeface="Consolas" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2091307792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2091307792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" charset="0"/>
+                    <a:ea typeface="Consolas" charset="0"/>
+                    <a:cs typeface="Consolas" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bandwidth(MHz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Consolas" charset="0"/>
+                  <a:ea typeface="Consolas" charset="0"/>
+                  <a:cs typeface="Consolas" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" charset="0"/>
+                <a:ea typeface="Consolas" charset="0"/>
+                <a:cs typeface="Consolas" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2096734560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="900">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="Consolas" charset="0"/>
+          <a:ea typeface="Consolas" charset="0"/>
+          <a:cs typeface="Consolas" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1039,10 +2337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:R14"/>
+  <dimension ref="A3:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="184" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A2" zoomScale="114" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1061,42 +2359,42 @@
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="23" t="s">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="23" t="s">
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="25"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="28"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="20"/>
@@ -1104,7 +2402,7 @@
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="M4" s="20"/>
@@ -1112,15 +2410,15 @@
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="22" t="s">
+      <c r="P4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="Q4" s="20"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1525,21 +2823,21 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="28"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="24"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
@@ -1596,6 +2894,12 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <f>I8/BCSR!N9</f>
+        <v>0.20105386512820933</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1615,4 +2919,656 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:P32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+    <col min="9" max="14" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="31"/>
+    </row>
+    <row r="6" spans="2:16" s="29" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="32">
+        <v>4</v>
+      </c>
+      <c r="C7" s="33">
+        <v>4</v>
+      </c>
+      <c r="D7" s="32">
+        <v>8192</v>
+      </c>
+      <c r="E7" s="32">
+        <v>100</v>
+      </c>
+      <c r="F7" s="34">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="G7" s="34">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H7" s="34">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="I7" s="33">
+        <v>5.0331599999999996</v>
+      </c>
+      <c r="J7" s="33">
+        <v>5.1649570000000002</v>
+      </c>
+      <c r="K7" s="33">
+        <v>9.6200000000000001E-3</v>
+      </c>
+      <c r="L7" s="33">
+        <v>106.667541935738</v>
+      </c>
+      <c r="M7" s="33">
+        <v>103.944895</v>
+      </c>
+      <c r="N7" s="33">
+        <v>0.20788999999999999</v>
+      </c>
+      <c r="O7" s="33">
+        <f>M7/L7</f>
+        <v>0.97447539442337328</v>
+      </c>
+      <c r="P7" s="33">
+        <f>N7/N7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="32"/>
+      <c r="C8" s="33">
+        <v>8</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="34">
+        <v>0.1137</v>
+      </c>
+      <c r="G8" s="34">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H8" s="34">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="I8" s="33">
+        <v>2.8311600000000001</v>
+      </c>
+      <c r="J8" s="33">
+        <v>3.0251169999999998</v>
+      </c>
+      <c r="K8" s="33">
+        <v>5.0090000000000004E-3</v>
+      </c>
+      <c r="L8" s="33">
+        <v>213.333541935738</v>
+      </c>
+      <c r="M8" s="33">
+        <v>199.65501399999999</v>
+      </c>
+      <c r="N8" s="33">
+        <v>0.39931</v>
+      </c>
+      <c r="O8" s="33">
+        <f t="shared" ref="O8:O13" si="0">M8/L8</f>
+        <v>0.93588196299736892</v>
+      </c>
+      <c r="P8" s="33">
+        <f>N8/$N$7</f>
+        <v>1.9207754100726346</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="32"/>
+      <c r="C9" s="33">
+        <v>16</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="34">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="G9" s="34">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H9" s="34">
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="I9" s="33">
+        <v>0.15728600000000001</v>
+      </c>
+      <c r="J9" s="33">
+        <v>0.45901599999999998</v>
+      </c>
+      <c r="K9" s="33">
+        <v>6.8399999999999997E-3</v>
+      </c>
+      <c r="L9" s="33">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="M9" s="33">
+        <v>244.053754</v>
+      </c>
+      <c r="N9" s="33">
+        <v>0.48810799999999999</v>
+      </c>
+      <c r="O9" s="33">
+        <f t="shared" si="0"/>
+        <v>0.57199981253028587</v>
+      </c>
+      <c r="P9" s="33">
+        <f t="shared" ref="P9:P13" si="1">N9/$N$7</f>
+        <v>2.3479147626148444</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="32"/>
+      <c r="C10" s="33">
+        <v>32</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="34">
+        <v>0.37890000000000001</v>
+      </c>
+      <c r="G10" s="34">
+        <v>0.127</v>
+      </c>
+      <c r="H10" s="34">
+        <v>0.57330000000000003</v>
+      </c>
+      <c r="I10" s="33">
+        <v>0.55050200000000005</v>
+      </c>
+      <c r="J10" s="33">
+        <v>1.939594</v>
+      </c>
+      <c r="K10" s="33">
+        <v>4.8170000000000001E-3</v>
+      </c>
+      <c r="L10" s="33">
+        <v>853.33354193573803</v>
+      </c>
+      <c r="M10" s="33">
+        <v>207.596633</v>
+      </c>
+      <c r="N10" s="33">
+        <v>0.41519299999999998</v>
+      </c>
+      <c r="O10" s="33">
+        <f t="shared" si="0"/>
+        <v>0.24327724482630669</v>
+      </c>
+      <c r="P10" s="33">
+        <f t="shared" si="1"/>
+        <v>1.9971763913608158</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="32">
+        <v>8</v>
+      </c>
+      <c r="C11" s="33">
+        <v>4</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="34">
+        <v>0.1166</v>
+      </c>
+      <c r="G11" s="34">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H11" s="34">
+        <v>0.15840000000000001</v>
+      </c>
+      <c r="I11" s="33">
+        <v>2.8311600000000001</v>
+      </c>
+      <c r="J11" s="33">
+        <v>3.0313699999999999</v>
+      </c>
+      <c r="K11" s="33">
+        <v>5.019E-3</v>
+      </c>
+      <c r="L11" s="33">
+        <v>213.333541935738</v>
+      </c>
+      <c r="M11" s="33">
+        <v>199.24317300000001</v>
+      </c>
+      <c r="N11" s="33">
+        <v>0.39848600000000001</v>
+      </c>
+      <c r="O11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.93395146019756048</v>
+      </c>
+      <c r="P11" s="33">
+        <f t="shared" si="1"/>
+        <v>1.916811775458175</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="32"/>
+      <c r="C12" s="33">
+        <v>8</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="34">
+        <v>0.2089</v>
+      </c>
+      <c r="G12" s="34">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H12" s="34">
+        <v>0.2979</v>
+      </c>
+      <c r="I12" s="33">
+        <v>1.4155800000000001</v>
+      </c>
+      <c r="J12" s="33">
+        <v>2.470313</v>
+      </c>
+      <c r="K12" s="33">
+        <v>4.0899999999999999E-3</v>
+      </c>
+      <c r="L12" s="33">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="M12" s="33">
+        <v>244.49524299999999</v>
+      </c>
+      <c r="N12" s="33">
+        <v>0.48898999999999998</v>
+      </c>
+      <c r="O12" s="33">
+        <f t="shared" si="0"/>
+        <v>0.57303455025136252</v>
+      </c>
+      <c r="P12" s="33">
+        <f t="shared" si="1"/>
+        <v>2.3521573909278946</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="32"/>
+      <c r="C13" s="33">
+        <v>16</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="34">
+        <v>0.37680000000000002</v>
+      </c>
+      <c r="G13" s="34">
+        <v>0.127</v>
+      </c>
+      <c r="H13" s="34">
+        <v>0.57709999999999995</v>
+      </c>
+      <c r="I13" s="33">
+        <v>0.62914599999999998</v>
+      </c>
+      <c r="J13" s="33">
+        <v>2.3740480000000002</v>
+      </c>
+      <c r="K13" s="33">
+        <v>4.4219999999999997E-3</v>
+      </c>
+      <c r="L13" s="33">
+        <v>853.33354193573803</v>
+      </c>
+      <c r="M13" s="33">
+        <v>226.14155700000001</v>
+      </c>
+      <c r="N13" s="33">
+        <v>0.45228299999999999</v>
+      </c>
+      <c r="O13" s="33">
+        <f t="shared" si="0"/>
+        <v>0.26500957232621009</v>
+      </c>
+      <c r="P13" s="33">
+        <f t="shared" si="1"/>
+        <v>2.1755880513733223</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="49"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="33">
+        <v>8192</v>
+      </c>
+      <c r="C25" s="44">
+        <v>8192</v>
+      </c>
+      <c r="D25" s="33">
+        <v>67108864</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0.15728600000000001</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0.457283</v>
+      </c>
+      <c r="G25" s="41">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="H25" s="40">
+        <v>146.75565</v>
+      </c>
+      <c r="I25" s="40">
+        <f>H25/H25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="33">
+        <v>16384</v>
+      </c>
+      <c r="C26" s="45"/>
+      <c r="D26" s="33">
+        <v>134217728</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0.31457299999999999</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0.72777099999999995</v>
+      </c>
+      <c r="G26" s="42"/>
+      <c r="H26" s="40">
+        <v>184.423023</v>
+      </c>
+      <c r="I26" s="40">
+        <f>H26/H25</f>
+        <v>1.2566672765239362</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="33">
+        <v>24576</v>
+      </c>
+      <c r="C27" s="45"/>
+      <c r="D27" s="33">
+        <v>201326592</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0.47185899999999997</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0.99838400000000005</v>
+      </c>
+      <c r="G27" s="42"/>
+      <c r="H27" s="40">
+        <v>201.65246200000001</v>
+      </c>
+      <c r="I27" s="40">
+        <f>H27/H25</f>
+        <v>1.3740694957911332</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="33">
+        <v>32768</v>
+      </c>
+      <c r="C28" s="45"/>
+      <c r="D28" s="33">
+        <v>268435456</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0.62914599999999998</v>
+      </c>
+      <c r="F28" s="33">
+        <v>1.2690570000000001</v>
+      </c>
+      <c r="G28" s="42"/>
+      <c r="H28" s="40">
+        <v>211.523561</v>
+      </c>
+      <c r="I28" s="40">
+        <f>H28/H25</f>
+        <v>1.4413316352726453</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="33">
+        <v>40960</v>
+      </c>
+      <c r="C29" s="45"/>
+      <c r="D29" s="33">
+        <v>335544320</v>
+      </c>
+      <c r="E29" s="33">
+        <v>0.78643200000000002</v>
+      </c>
+      <c r="F29" s="33">
+        <v>1.5138590000000001</v>
+      </c>
+      <c r="G29" s="42"/>
+      <c r="H29" s="40">
+        <v>221.64833100000001</v>
+      </c>
+      <c r="I29" s="40">
+        <f>H29/H25</f>
+        <v>1.5103223010493976</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="33">
+        <v>49152</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="33">
+        <v>402653184</v>
+      </c>
+      <c r="E30" s="33">
+        <v>0.94371799999999995</v>
+      </c>
+      <c r="F30" s="33">
+        <v>1.756033</v>
+      </c>
+      <c r="G30" s="42"/>
+      <c r="H30" s="40">
+        <v>229.29704899999999</v>
+      </c>
+      <c r="I30" s="40">
+        <f>H30/H25</f>
+        <v>1.5624410303794094</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="33">
+        <v>57344</v>
+      </c>
+      <c r="C31" s="45"/>
+      <c r="D31" s="33">
+        <v>469762048</v>
+      </c>
+      <c r="E31" s="33">
+        <v>1.101</v>
+      </c>
+      <c r="F31" s="33">
+        <v>1.9886269999999999</v>
+      </c>
+      <c r="G31" s="42"/>
+      <c r="H31" s="40">
+        <v>236.22431399999999</v>
+      </c>
+      <c r="I31" s="40">
+        <f>H31/H25</f>
+        <v>1.6096437445508911</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="33">
+        <v>65536</v>
+      </c>
+      <c r="C32" s="46"/>
+      <c r="D32" s="33">
+        <v>536870912</v>
+      </c>
+      <c r="E32" s="33">
+        <v>1.2582899999999999</v>
+      </c>
+      <c r="F32" s="33">
+        <v>2.1998060000000002</v>
+      </c>
+      <c r="G32" s="43"/>
+      <c r="H32" s="40">
+        <v>244.053754</v>
+      </c>
+      <c r="I32" s="40">
+        <f>H32/H25</f>
+        <v>1.66299392221015</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="C25:C32"/>
+    <mergeCell ref="G25:G32"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="E7:E13"/>
+    <mergeCell ref="F5:H5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated week 4 report
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -410,65 +410,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,15 +478,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,6 +486,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -743,11 +743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2096734560"/>
-        <c:axId val="-2091307792"/>
+        <c:axId val="2128646752"/>
+        <c:axId val="2128655152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2096734560"/>
+        <c:axId val="2128646752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,7 +856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091307792"/>
+        <c:crossAx val="2128655152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +864,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2091307792"/>
+        <c:axId val="2128655152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +962,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096734560"/>
+        <c:crossAx val="2128646752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1914,23 +1914,23 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="N2" s="20" t="s">
+      <c r="H2" s="26"/>
+      <c r="N2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1981,10 +1981,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="27">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -2005,10 +2005,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="29">
         <v>8192</v>
       </c>
-      <c r="O4" s="21">
+      <c r="O4" s="29">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -2029,8 +2029,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -2049,8 +2049,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -2069,8 +2069,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -2089,8 +2089,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -2109,8 +2109,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -2129,8 +2129,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21">
+      <c r="N7" s="29"/>
+      <c r="O7" s="29">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -2151,8 +2151,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -2171,8 +2171,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -2191,8 +2191,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N10" s="21"/>
-      <c r="O10" s="21">
+      <c r="N10" s="29"/>
+      <c r="O10" s="29">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -2213,8 +2213,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -2233,8 +2233,8 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -2253,8 +2253,8 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N13" s="21"/>
-      <c r="O13" s="21">
+      <c r="N13" s="29"/>
+      <c r="O13" s="29">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -2275,8 +2275,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -2295,8 +2295,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -2353,72 +2353,72 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="26" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="26" t="s">
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="28"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="36"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="28"/>
       <c r="J4" s="2"/>
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="20"/>
+      <c r="M4" s="28"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="20"/>
+      <c r="Q4" s="28"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="21">
+      <c r="A6" s="29">
         <v>8192</v>
       </c>
       <c r="B6" s="6">
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -2582,7 +2582,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -2639,7 +2639,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -2696,7 +2696,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="7">
         <v>16</v>
       </c>
@@ -2753,7 +2753,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="7">
         <v>32</v>
       </c>
@@ -2810,7 +2810,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="7">
         <v>64</v>
       </c>
@@ -2823,24 +2823,24 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="24"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="32"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="7">
         <v>128</v>
       </c>
@@ -2868,7 +2868,7 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="7">
         <v>256</v>
       </c>
@@ -2925,8 +2925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2941,620 +2941,924 @@
     <col min="9" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="35" t="s">
+    <row r="5" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="36" t="s">
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="35" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="31"/>
-    </row>
-    <row r="6" spans="2:16" s="29" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="P5" s="48"/>
+    </row>
+    <row r="6" spans="2:16" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="37" t="s">
+      <c r="O6" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="P6" s="37" t="s">
+      <c r="P6" s="22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="32">
+    <row r="7" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="49">
         <v>4</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="20">
         <v>4</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="49">
         <v>8192</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="49">
         <v>100</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="21">
         <v>7.0800000000000002E-2</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="21">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="21">
         <v>8.5099999999999995E-2</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="20">
         <v>5.0331599999999996</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="20">
         <v>5.1649570000000002</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="20">
         <v>9.6200000000000001E-3</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="20">
         <v>106.667541935738</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="20">
         <v>103.944895</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="20">
         <v>0.20788999999999999</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="20">
         <f>M7/L7</f>
         <v>0.97447539442337328</v>
       </c>
-      <c r="P7" s="33">
+      <c r="P7" s="20">
         <f>N7/N7</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="32"/>
-      <c r="C8" s="33">
+    <row r="8" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="49"/>
+      <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="34">
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="21">
         <v>0.1137</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="21">
         <v>3.1699999999999999E-2</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="21">
         <v>0.15509999999999999</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="20">
         <v>2.8311600000000001</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="20">
         <v>3.0251169999999998</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="20">
         <v>5.0090000000000004E-3</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="20">
         <v>213.333541935738</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="20">
         <v>199.65501399999999</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="20">
         <v>0.39931</v>
       </c>
-      <c r="O8" s="33">
+      <c r="O8" s="20">
         <f t="shared" ref="O8:O13" si="0">M8/L8</f>
         <v>0.93588196299736892</v>
       </c>
-      <c r="P8" s="33">
+      <c r="P8" s="20">
         <f>N8/$N$7</f>
         <v>1.9207754100726346</v>
       </c>
     </row>
-    <row r="9" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="32"/>
-      <c r="C9" s="33">
+    <row r="9" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="49"/>
+      <c r="C9" s="20">
         <v>16</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="34">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="21">
         <v>0.20280000000000001</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="21">
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="21">
         <v>0.29420000000000002</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="20">
         <v>0.15728600000000001</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="20">
         <v>0.45901599999999998</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="20">
         <v>6.8399999999999997E-3</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="20">
         <v>426.66754193573797</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="20">
         <v>244.053754</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="20">
         <v>0.48810799999999999</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="20">
         <f t="shared" si="0"/>
         <v>0.57199981253028587</v>
       </c>
-      <c r="P9" s="33">
+      <c r="P9" s="20">
         <f t="shared" ref="P9:P13" si="1">N9/$N$7</f>
         <v>2.3479147626148444</v>
       </c>
     </row>
-    <row r="10" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="32"/>
-      <c r="C10" s="33">
+    <row r="10" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="49"/>
+      <c r="C10" s="20">
         <v>32</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="34">
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="21">
         <v>0.37890000000000001</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="21">
         <v>0.127</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="21">
         <v>0.57330000000000003</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="20">
         <v>0.55050200000000005</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="20">
         <v>1.939594</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="20">
         <v>4.8170000000000001E-3</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="20">
         <v>853.33354193573803</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="20">
         <v>207.596633</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="20">
         <v>0.41519299999999998</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="20">
         <f t="shared" si="0"/>
         <v>0.24327724482630669</v>
       </c>
-      <c r="P10" s="33">
+      <c r="P10" s="20">
         <f t="shared" si="1"/>
         <v>1.9971763913608158</v>
       </c>
     </row>
-    <row r="11" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="32">
+    <row r="11" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="49">
         <v>8</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="34">
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="21">
         <v>0.1166</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="21">
         <v>3.1699999999999999E-2</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="21">
         <v>0.15840000000000001</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="20">
         <v>2.8311600000000001</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="20">
         <v>3.0313699999999999</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="20">
         <v>5.019E-3</v>
       </c>
-      <c r="L11" s="33">
+      <c r="L11" s="20">
         <v>213.333541935738</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="20">
         <v>199.24317300000001</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="20">
         <v>0.39848600000000001</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="20">
         <f t="shared" si="0"/>
         <v>0.93395146019756048</v>
       </c>
-      <c r="P11" s="33">
+      <c r="P11" s="20">
         <f t="shared" si="1"/>
         <v>1.916811775458175</v>
       </c>
     </row>
-    <row r="12" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="32"/>
-      <c r="C12" s="33">
+    <row r="12" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="49"/>
+      <c r="C12" s="20">
         <v>8</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="34">
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="21">
         <v>0.2089</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="21">
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="H12" s="34">
+      <c r="H12" s="21">
         <v>0.2979</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="20">
         <v>1.4155800000000001</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="20">
         <v>2.470313</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="20">
         <v>4.0899999999999999E-3</v>
       </c>
-      <c r="L12" s="33">
+      <c r="L12" s="20">
         <v>426.66754193573797</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="20">
         <v>244.49524299999999</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="20">
         <v>0.48898999999999998</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="20">
         <f t="shared" si="0"/>
         <v>0.57303455025136252</v>
       </c>
-      <c r="P12" s="33">
+      <c r="P12" s="20">
         <f t="shared" si="1"/>
         <v>2.3521573909278946</v>
       </c>
     </row>
-    <row r="13" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="32"/>
-      <c r="C13" s="33">
+    <row r="13" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="49"/>
+      <c r="C13" s="20">
         <v>16</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="34">
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="21">
         <v>0.37680000000000002</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="21">
         <v>0.127</v>
       </c>
-      <c r="H13" s="34">
+      <c r="H13" s="21">
         <v>0.57709999999999995</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="20">
         <v>0.62914599999999998</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="20">
         <v>2.3740480000000002</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="20">
         <v>4.4219999999999997E-3</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="20">
         <v>853.33354193573803</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="20">
         <v>226.14155700000001</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="20">
         <v>0.45228299999999999</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="20">
         <f t="shared" si="0"/>
         <v>0.26500957232621009</v>
       </c>
-      <c r="P13" s="33">
+      <c r="P13" s="20">
         <f t="shared" si="1"/>
         <v>2.1755880513733223</v>
       </c>
     </row>
-    <row r="14" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="2:16" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:9" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="47" t="s">
+    <row r="14" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="49">
+        <v>4</v>
+      </c>
+      <c r="C14" s="20">
+        <v>4</v>
+      </c>
+      <c r="D14" s="49">
+        <v>8192</v>
+      </c>
+      <c r="E14" s="49">
+        <v>150</v>
+      </c>
+      <c r="F14" s="21">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="G14" s="21">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H14" s="21">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="I14" s="20">
+        <v>5.0331599999999996</v>
+      </c>
+      <c r="J14" s="20">
+        <v>5.1649570000000002</v>
+      </c>
+      <c r="K14" s="20">
+        <v>9.6200000000000001E-3</v>
+      </c>
+      <c r="L14" s="20">
+        <v>106.667541935738</v>
+      </c>
+      <c r="M14" s="20">
+        <v>103.944895</v>
+      </c>
+      <c r="N14" s="20">
+        <v>0.20788999999999999</v>
+      </c>
+      <c r="O14" s="20">
+        <f>M14/L14</f>
+        <v>0.97447539442337328</v>
+      </c>
+      <c r="P14" s="20">
+        <f>N14/N14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="49"/>
+      <c r="C15" s="20">
+        <v>8</v>
+      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="21">
+        <v>0.1137</v>
+      </c>
+      <c r="G15" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H15" s="21">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="I15" s="20">
+        <v>2.8311600000000001</v>
+      </c>
+      <c r="J15" s="20">
+        <v>3.0251169999999998</v>
+      </c>
+      <c r="K15" s="20">
+        <v>5.0090000000000004E-3</v>
+      </c>
+      <c r="L15" s="20">
+        <v>213.333541935738</v>
+      </c>
+      <c r="M15" s="20">
+        <v>199.65501399999999</v>
+      </c>
+      <c r="N15" s="20">
+        <v>0.39931</v>
+      </c>
+      <c r="O15" s="20">
+        <f t="shared" ref="O15:O20" si="2">M15/L15</f>
+        <v>0.93588196299736892</v>
+      </c>
+      <c r="P15" s="20">
+        <f>N15/$N$7</f>
+        <v>1.9207754100726346</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="49"/>
+      <c r="C16" s="20">
+        <v>16</v>
+      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="21">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="G16" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H16" s="21">
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="I16" s="20">
+        <v>0.15728600000000001</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0.45901599999999998</v>
+      </c>
+      <c r="K16" s="20">
+        <v>6.8399999999999997E-3</v>
+      </c>
+      <c r="L16" s="20">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="M16" s="20">
+        <v>244.053754</v>
+      </c>
+      <c r="N16" s="20">
+        <v>0.48810799999999999</v>
+      </c>
+      <c r="O16" s="20">
+        <f t="shared" si="2"/>
+        <v>0.57199981253028587</v>
+      </c>
+      <c r="P16" s="20">
+        <f t="shared" ref="P16:P20" si="3">N16/$N$7</f>
+        <v>2.3479147626148444</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="49"/>
+      <c r="C17" s="20">
+        <v>32</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="21">
+        <v>0.37890000000000001</v>
+      </c>
+      <c r="G17" s="21">
+        <v>0.127</v>
+      </c>
+      <c r="H17" s="21">
+        <v>0.57330000000000003</v>
+      </c>
+      <c r="I17" s="20">
+        <v>0.55050200000000005</v>
+      </c>
+      <c r="J17" s="20">
+        <v>1.939594</v>
+      </c>
+      <c r="K17" s="20">
+        <v>4.8170000000000001E-3</v>
+      </c>
+      <c r="L17" s="20">
+        <v>853.33354193573803</v>
+      </c>
+      <c r="M17" s="20">
+        <v>207.596633</v>
+      </c>
+      <c r="N17" s="20">
+        <v>0.41519299999999998</v>
+      </c>
+      <c r="O17" s="20">
+        <f t="shared" si="2"/>
+        <v>0.24327724482630669</v>
+      </c>
+      <c r="P17" s="20">
+        <f t="shared" si="3"/>
+        <v>1.9971763913608158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="49">
+        <v>8</v>
+      </c>
+      <c r="C18" s="20">
+        <v>4</v>
+      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="21">
+        <v>0.1166</v>
+      </c>
+      <c r="G18" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H18" s="21">
+        <v>0.15840000000000001</v>
+      </c>
+      <c r="I18" s="20">
+        <v>2.8311600000000001</v>
+      </c>
+      <c r="J18" s="20">
+        <v>3.0313699999999999</v>
+      </c>
+      <c r="K18" s="20">
+        <v>5.019E-3</v>
+      </c>
+      <c r="L18" s="20">
+        <v>213.333541935738</v>
+      </c>
+      <c r="M18" s="20">
+        <v>199.24317300000001</v>
+      </c>
+      <c r="N18" s="20">
+        <v>0.39848600000000001</v>
+      </c>
+      <c r="O18" s="20">
+        <f t="shared" si="2"/>
+        <v>0.93395146019756048</v>
+      </c>
+      <c r="P18" s="20">
+        <f t="shared" si="3"/>
+        <v>1.916811775458175</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B19" s="49"/>
+      <c r="C19" s="20">
+        <v>8</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="21">
+        <v>0.2089</v>
+      </c>
+      <c r="G19" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H19" s="21">
+        <v>0.2979</v>
+      </c>
+      <c r="I19" s="20">
+        <v>1.4155800000000001</v>
+      </c>
+      <c r="J19" s="20">
+        <v>2.470313</v>
+      </c>
+      <c r="K19" s="20">
+        <v>4.0899999999999999E-3</v>
+      </c>
+      <c r="L19" s="20">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="M19" s="20">
+        <v>244.49524299999999</v>
+      </c>
+      <c r="N19" s="20">
+        <v>0.48898999999999998</v>
+      </c>
+      <c r="O19" s="20">
+        <f t="shared" si="2"/>
+        <v>0.57303455025136252</v>
+      </c>
+      <c r="P19" s="20">
+        <f t="shared" si="3"/>
+        <v>2.3521573909278946</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="49"/>
+      <c r="C20" s="20">
+        <v>16</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="21">
+        <v>0.37680000000000002</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0.127</v>
+      </c>
+      <c r="H20" s="21">
+        <v>0.57709999999999995</v>
+      </c>
+      <c r="I20" s="20">
+        <v>0.62914599999999998</v>
+      </c>
+      <c r="J20" s="20">
+        <v>2.3740480000000002</v>
+      </c>
+      <c r="K20" s="20">
+        <v>4.4219999999999997E-3</v>
+      </c>
+      <c r="L20" s="20">
+        <v>853.33354193573803</v>
+      </c>
+      <c r="M20" s="20">
+        <v>226.14155700000001</v>
+      </c>
+      <c r="N20" s="20">
+        <v>0.45228299999999999</v>
+      </c>
+      <c r="O20" s="20">
+        <f t="shared" si="2"/>
+        <v>0.26500957232621009</v>
+      </c>
+      <c r="P20" s="20">
+        <f t="shared" si="3"/>
+        <v>2.1755880513733223</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B23" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="49"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="39" t="s">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H24" s="39" t="s">
+      <c r="H24" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="33">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B25" s="20">
         <v>8192</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="38">
         <v>8192</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D25" s="20">
         <v>67108864</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="20">
         <v>0.15728600000000001</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="20">
         <v>0.457283</v>
       </c>
       <c r="G25" s="41">
         <v>426.66754193573797</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="25">
         <v>146.75565</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="25">
         <f>H25/H25</f>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="33">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B26" s="20">
         <v>16384</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="33">
+      <c r="C26" s="39"/>
+      <c r="D26" s="20">
         <v>134217728</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="20">
         <v>0.31457299999999999</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="20">
         <v>0.72777099999999995</v>
       </c>
       <c r="G26" s="42"/>
-      <c r="H26" s="40">
+      <c r="H26" s="25">
         <v>184.423023</v>
       </c>
-      <c r="I26" s="40">
+      <c r="I26" s="25">
         <f>H26/H25</f>
         <v>1.2566672765239362</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="33">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B27" s="20">
         <v>24576</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="33">
+      <c r="C27" s="39"/>
+      <c r="D27" s="20">
         <v>201326592</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="20">
         <v>0.47185899999999997</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="20">
         <v>0.99838400000000005</v>
       </c>
       <c r="G27" s="42"/>
-      <c r="H27" s="40">
+      <c r="H27" s="25">
         <v>201.65246200000001</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="25">
         <f>H27/H25</f>
         <v>1.3740694957911332</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="33">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B28" s="20">
         <v>32768</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="33">
+      <c r="C28" s="39"/>
+      <c r="D28" s="20">
         <v>268435456</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="20">
         <v>0.62914599999999998</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="20">
         <v>1.2690570000000001</v>
       </c>
       <c r="G28" s="42"/>
-      <c r="H28" s="40">
+      <c r="H28" s="25">
         <v>211.523561</v>
       </c>
-      <c r="I28" s="40">
+      <c r="I28" s="25">
         <f>H28/H25</f>
         <v>1.4413316352726453</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="33">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="20">
         <v>40960</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="33">
+      <c r="C29" s="39"/>
+      <c r="D29" s="20">
         <v>335544320</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="20">
         <v>0.78643200000000002</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="20">
         <v>1.5138590000000001</v>
       </c>
       <c r="G29" s="42"/>
-      <c r="H29" s="40">
+      <c r="H29" s="25">
         <v>221.64833100000001</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="25">
         <f>H29/H25</f>
         <v>1.5103223010493976</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="33">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B30" s="20">
         <v>49152</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="33">
+      <c r="C30" s="39"/>
+      <c r="D30" s="20">
         <v>402653184</v>
       </c>
-      <c r="E30" s="33">
+      <c r="E30" s="20">
         <v>0.94371799999999995</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="20">
         <v>1.756033</v>
       </c>
       <c r="G30" s="42"/>
-      <c r="H30" s="40">
+      <c r="H30" s="25">
         <v>229.29704899999999</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="25">
         <f>H30/H25</f>
         <v>1.5624410303794094</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="33">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B31" s="20">
         <v>57344</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="33">
+      <c r="C31" s="39"/>
+      <c r="D31" s="20">
         <v>469762048</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="20">
         <v>1.101</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="20">
         <v>1.9886269999999999</v>
       </c>
       <c r="G31" s="42"/>
-      <c r="H31" s="40">
+      <c r="H31" s="25">
         <v>236.22431399999999</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="25">
         <f>H31/H25</f>
         <v>1.6096437445508911</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="33">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B32" s="20">
         <v>65536</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="33">
+      <c r="C32" s="40"/>
+      <c r="D32" s="20">
         <v>536870912</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="20">
         <v>1.2582899999999999</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="20">
         <v>2.1998060000000002</v>
       </c>
       <c r="G32" s="43"/>
-      <c r="H32" s="40">
+      <c r="H32" s="25">
         <v>244.053754</v>
       </c>
-      <c r="I32" s="40">
+      <c r="I32" s="25">
         <f>H32/H25</f>
         <v>1.66299392221015</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="C25:C32"/>
     <mergeCell ref="G25:G32"/>
@@ -3566,6 +3870,10 @@
     <mergeCell ref="D7:D13"/>
     <mergeCell ref="E7:E13"/>
     <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="D14:D20"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated with latest SpMV version
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
   <si>
     <t>numPipes</t>
   </si>
@@ -131,68 +131,96 @@
     <t>Resource Usage</t>
   </si>
   <si>
-    <t>Multipliers</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Estimated
-Time(s)</t>
-  </si>
-  <si>
-    <t>Total
-Time(s)</t>
-  </si>
-  <si>
     <t>Time per
 element(us)</t>
   </si>
   <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Dense Matrix: Special study on 4 X 16 block with 8192 ROM size</t>
+  </si>
+  <si>
+    <t>nnz</t>
+  </si>
+  <si>
+    <t>Esti. Time</t>
+  </si>
+  <si>
+    <t>Esti. Band</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Comp to 1.</t>
+  </si>
+  <si>
+    <t>Frequency
+(MHz)</t>
+  </si>
+  <si>
     <t>Bandwidth
-(MHz)</t>
-  </si>
-  <si>
-    <t>Estimated
-Bandwidth(MHz)</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>Dense Matrix: Special study on 4 X 16 block with 8192 ROM size</t>
-  </si>
-  <si>
-    <t>nnz</t>
-  </si>
-  <si>
-    <t>Esti. Time</t>
-  </si>
-  <si>
-    <t>Esti. Band</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Band</t>
-  </si>
-  <si>
-    <t>Real/Esti.</t>
-  </si>
-  <si>
-    <t>Comp to 1.</t>
+(MB/s)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Experiment data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>w/o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> C-Slowing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Experiment data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>w/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> C-Slowing(L=16)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -365,7 +393,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -417,13 +445,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,6 +527,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -667,7 +704,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>BCSR!$B$25:$B$32</c:f>
+              <c:f>BCSR!$O$7:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -700,7 +737,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BCSR!$H$25:$H$32</c:f>
+              <c:f>BCSR!$U$7:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -743,11 +780,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2128646752"/>
-        <c:axId val="2128655152"/>
+        <c:axId val="-2120314704"/>
+        <c:axId val="-2131183280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2128646752"/>
+        <c:axId val="-2120314704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,7 +893,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128655152"/>
+        <c:crossAx val="-2131183280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128655152"/>
+        <c:axId val="-2131183280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128646752"/>
+        <c:crossAx val="-2120314704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1578,16 +1615,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>458611</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>117592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>431330</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>94543</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1914,23 +1951,23 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="N2" s="28" t="s">
+      <c r="H2" s="27"/>
+      <c r="N2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1981,10 +2018,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="28">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -2005,10 +2042,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="30">
         <v>8192</v>
       </c>
-      <c r="O4" s="29">
+      <c r="O4" s="30">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -2029,8 +2066,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -2049,8 +2086,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -2069,8 +2106,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -2089,8 +2126,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -2109,8 +2146,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -2129,8 +2166,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29">
+      <c r="N7" s="30"/>
+      <c r="O7" s="30">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -2151,8 +2188,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -2171,8 +2208,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -2191,8 +2228,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N10" s="29"/>
-      <c r="O10" s="29">
+      <c r="N10" s="30"/>
+      <c r="O10" s="30">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -2213,8 +2250,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -2233,8 +2270,8 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -2253,8 +2290,8 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N13" s="29"/>
-      <c r="O13" s="29">
+      <c r="N13" s="30"/>
+      <c r="O13" s="30">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -2275,8 +2312,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -2295,8 +2332,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -2340,7 +2377,7 @@
   <dimension ref="A3:R24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="114" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2353,72 +2390,72 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="34" t="s">
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="34" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="37"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="28"/>
+      <c r="I4" s="29"/>
       <c r="J4" s="2"/>
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="28"/>
+      <c r="M4" s="29"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="28"/>
+      <c r="Q4" s="29"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +2506,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="29">
+      <c r="A6" s="30">
         <v>8192</v>
       </c>
       <c r="B6" s="6">
@@ -2525,7 +2562,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -2582,7 +2619,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -2639,7 +2676,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -2696,7 +2733,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="7">
         <v>16</v>
       </c>
@@ -2753,7 +2790,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="7">
         <v>32</v>
       </c>
@@ -2810,7 +2847,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="7">
         <v>64</v>
       </c>
@@ -2823,24 +2860,24 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="33"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="7">
         <v>128</v>
       </c>
@@ -2868,7 +2905,7 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="7">
         <v>256</v>
       </c>
@@ -2897,7 +2934,7 @@
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E24">
-        <f>I8/BCSR!N9</f>
+        <f>I8/BCSR!L9</f>
         <v>0.20105386512820933</v>
       </c>
     </row>
@@ -2923,10 +2960,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:P32"/>
+  <dimension ref="B4:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="108" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2936,94 +2973,128 @@
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" customWidth="1"/>
-    <col min="9" max="14" width="12" customWidth="1"/>
+    <col min="9" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="47" t="s">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B4" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+    </row>
+    <row r="5" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="37" t="s">
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="26"/>
+      <c r="O5" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="47"/>
+    </row>
+    <row r="6" spans="2:22" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="47" t="s">
+      <c r="P6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="48"/>
-    </row>
-    <row r="6" spans="2:16" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="49">
+    </row>
+    <row r="7" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="50">
         <v>4</v>
       </c>
       <c r="C7" s="20">
         <v>4</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="50">
         <v>8192</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="50">
         <v>100</v>
       </c>
       <c r="F7" s="21">
@@ -3036,39 +3107,56 @@
         <v>8.5099999999999995E-2</v>
       </c>
       <c r="I7" s="20">
-        <v>5.0331599999999996</v>
+        <v>9.6200000000000001E-3</v>
       </c>
       <c r="J7" s="20">
-        <v>5.1649570000000002</v>
+        <f>1/I7</f>
+        <v>103.95010395010395</v>
       </c>
       <c r="K7" s="20">
-        <v>9.6200000000000001E-3</v>
+        <f>4/I7</f>
+        <v>415.80041580041581</v>
       </c>
       <c r="L7" s="20">
-        <v>106.667541935738</v>
+        <v>0.20788999999999999</v>
       </c>
       <c r="M7" s="20">
-        <v>103.944895</v>
-      </c>
-      <c r="N7" s="20">
-        <v>0.20788999999999999</v>
+        <f>L7/L7</f>
+        <v>1</v>
       </c>
       <c r="O7" s="20">
-        <f>M7/L7</f>
-        <v>0.97447539442337328</v>
-      </c>
-      <c r="P7" s="20">
-        <f>N7/N7</f>
+        <v>8192</v>
+      </c>
+      <c r="P7" s="39">
+        <v>8192</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>67108864</v>
+      </c>
+      <c r="R7" s="20">
+        <v>0.15728600000000001</v>
+      </c>
+      <c r="S7" s="20">
+        <v>0.457283</v>
+      </c>
+      <c r="T7" s="42">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="U7" s="24">
+        <v>146.75565</v>
+      </c>
+      <c r="V7" s="24">
+        <f>U7/U7</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="49"/>
+    <row r="8" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="50"/>
       <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="21">
         <v>0.1137</v>
       </c>
@@ -3079,39 +3167,52 @@
         <v>0.15509999999999999</v>
       </c>
       <c r="I8" s="20">
-        <v>2.8311600000000001</v>
+        <v>5.0090000000000004E-3</v>
       </c>
       <c r="J8" s="20">
-        <v>3.0251169999999998</v>
+        <f t="shared" ref="J8:J13" si="0">1/I8</f>
+        <v>199.64064683569572</v>
       </c>
       <c r="K8" s="20">
-        <v>5.0090000000000004E-3</v>
+        <f t="shared" ref="K8:K13" si="1">4/I8</f>
+        <v>798.56258734278288</v>
       </c>
       <c r="L8" s="20">
-        <v>213.333541935738</v>
+        <v>0.39931</v>
       </c>
       <c r="M8" s="20">
-        <v>199.65501399999999</v>
-      </c>
-      <c r="N8" s="20">
-        <v>0.39931</v>
+        <f>L8/$L$7</f>
+        <v>1.9207754100726346</v>
       </c>
       <c r="O8" s="20">
-        <f t="shared" ref="O8:O13" si="0">M8/L8</f>
-        <v>0.93588196299736892</v>
-      </c>
-      <c r="P8" s="20">
-        <f>N8/$N$7</f>
-        <v>1.9207754100726346</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="49"/>
+        <v>16384</v>
+      </c>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="20">
+        <v>134217728</v>
+      </c>
+      <c r="R8" s="20">
+        <v>0.31457299999999999</v>
+      </c>
+      <c r="S8" s="20">
+        <v>0.72777099999999995</v>
+      </c>
+      <c r="T8" s="43"/>
+      <c r="U8" s="24">
+        <v>184.423023</v>
+      </c>
+      <c r="V8" s="24">
+        <f>U8/U7</f>
+        <v>1.2566672765239362</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="50"/>
       <c r="C9" s="20">
         <v>16</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="21">
         <v>0.20280000000000001</v>
       </c>
@@ -3122,39 +3223,52 @@
         <v>0.29420000000000002</v>
       </c>
       <c r="I9" s="20">
-        <v>0.15728600000000001</v>
+        <v>6.8399999999999997E-3</v>
       </c>
       <c r="J9" s="20">
-        <v>0.45901599999999998</v>
+        <f t="shared" si="0"/>
+        <v>146.19883040935673</v>
       </c>
       <c r="K9" s="20">
-        <v>6.8399999999999997E-3</v>
+        <f t="shared" si="1"/>
+        <v>584.79532163742692</v>
       </c>
       <c r="L9" s="20">
-        <v>426.66754193573797</v>
+        <v>0.48810799999999999</v>
       </c>
       <c r="M9" s="20">
-        <v>244.053754</v>
-      </c>
-      <c r="N9" s="20">
-        <v>0.48810799999999999</v>
+        <f t="shared" ref="M9:M13" si="2">L9/$L$7</f>
+        <v>2.3479147626148444</v>
       </c>
       <c r="O9" s="20">
-        <f t="shared" si="0"/>
-        <v>0.57199981253028587</v>
-      </c>
-      <c r="P9" s="20">
-        <f t="shared" ref="P9:P13" si="1">N9/$N$7</f>
-        <v>2.3479147626148444</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="49"/>
+        <v>24576</v>
+      </c>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="20">
+        <v>201326592</v>
+      </c>
+      <c r="R9" s="20">
+        <v>0.47185899999999997</v>
+      </c>
+      <c r="S9" s="20">
+        <v>0.99838400000000005</v>
+      </c>
+      <c r="T9" s="43"/>
+      <c r="U9" s="24">
+        <v>201.65246200000001</v>
+      </c>
+      <c r="V9" s="24">
+        <f>U9/U7</f>
+        <v>1.3740694957911332</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="50"/>
       <c r="C10" s="20">
         <v>32</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="21">
         <v>0.37890000000000001</v>
       </c>
@@ -3165,41 +3279,54 @@
         <v>0.57330000000000003</v>
       </c>
       <c r="I10" s="20">
-        <v>0.55050200000000005</v>
+        <v>4.8170000000000001E-3</v>
       </c>
       <c r="J10" s="20">
-        <v>1.939594</v>
+        <f t="shared" si="0"/>
+        <v>207.59809009757109</v>
       </c>
       <c r="K10" s="20">
-        <v>4.8170000000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>830.39236039028435</v>
       </c>
       <c r="L10" s="20">
-        <v>853.33354193573803</v>
+        <v>0.41519299999999998</v>
       </c>
       <c r="M10" s="20">
-        <v>207.596633</v>
-      </c>
-      <c r="N10" s="20">
-        <v>0.41519299999999998</v>
+        <f t="shared" si="2"/>
+        <v>1.9971763913608158</v>
       </c>
       <c r="O10" s="20">
-        <f t="shared" si="0"/>
-        <v>0.24327724482630669</v>
-      </c>
-      <c r="P10" s="20">
-        <f t="shared" si="1"/>
-        <v>1.9971763913608158</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="49">
+        <v>32768</v>
+      </c>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="20">
+        <v>268435456</v>
+      </c>
+      <c r="R10" s="20">
+        <v>0.62914599999999998</v>
+      </c>
+      <c r="S10" s="20">
+        <v>1.2690570000000001</v>
+      </c>
+      <c r="T10" s="43"/>
+      <c r="U10" s="24">
+        <v>211.523561</v>
+      </c>
+      <c r="V10" s="24">
+        <f>U10/U7</f>
+        <v>1.4413316352726453</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="50">
         <v>8</v>
       </c>
       <c r="C11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="21">
         <v>0.1166</v>
       </c>
@@ -3210,39 +3337,52 @@
         <v>0.15840000000000001</v>
       </c>
       <c r="I11" s="20">
-        <v>2.8311600000000001</v>
+        <v>5.019E-3</v>
       </c>
       <c r="J11" s="20">
-        <v>3.0313699999999999</v>
+        <f t="shared" si="0"/>
+        <v>199.24287706714486</v>
       </c>
       <c r="K11" s="20">
-        <v>5.019E-3</v>
+        <f t="shared" si="1"/>
+        <v>796.97150826857944</v>
       </c>
       <c r="L11" s="20">
-        <v>213.333541935738</v>
+        <v>0.39848600000000001</v>
       </c>
       <c r="M11" s="20">
-        <v>199.24317300000001</v>
-      </c>
-      <c r="N11" s="20">
-        <v>0.39848600000000001</v>
+        <f t="shared" si="2"/>
+        <v>1.916811775458175</v>
       </c>
       <c r="O11" s="20">
-        <f t="shared" si="0"/>
-        <v>0.93395146019756048</v>
-      </c>
-      <c r="P11" s="20">
-        <f t="shared" si="1"/>
-        <v>1.916811775458175</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="49"/>
+        <v>40960</v>
+      </c>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="20">
+        <v>335544320</v>
+      </c>
+      <c r="R11" s="20">
+        <v>0.78643200000000002</v>
+      </c>
+      <c r="S11" s="20">
+        <v>1.5138590000000001</v>
+      </c>
+      <c r="T11" s="43"/>
+      <c r="U11" s="24">
+        <v>221.64833100000001</v>
+      </c>
+      <c r="V11" s="24">
+        <f>U11/U7</f>
+        <v>1.5103223010493976</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="50"/>
       <c r="C12" s="20">
         <v>8</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="21">
         <v>0.2089</v>
       </c>
@@ -3253,39 +3393,52 @@
         <v>0.2979</v>
       </c>
       <c r="I12" s="20">
-        <v>1.4155800000000001</v>
+        <v>4.0899999999999999E-3</v>
       </c>
       <c r="J12" s="20">
-        <v>2.470313</v>
+        <f t="shared" si="0"/>
+        <v>244.49877750611248</v>
       </c>
       <c r="K12" s="20">
-        <v>4.0899999999999999E-3</v>
+        <f t="shared" si="1"/>
+        <v>977.9951100244499</v>
       </c>
       <c r="L12" s="20">
-        <v>426.66754193573797</v>
+        <v>0.48898999999999998</v>
       </c>
       <c r="M12" s="20">
-        <v>244.49524299999999</v>
-      </c>
-      <c r="N12" s="20">
-        <v>0.48898999999999998</v>
+        <f t="shared" si="2"/>
+        <v>2.3521573909278946</v>
       </c>
       <c r="O12" s="20">
-        <f t="shared" si="0"/>
-        <v>0.57303455025136252</v>
-      </c>
-      <c r="P12" s="20">
-        <f t="shared" si="1"/>
-        <v>2.3521573909278946</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="49"/>
+        <v>49152</v>
+      </c>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="20">
+        <v>402653184</v>
+      </c>
+      <c r="R12" s="20">
+        <v>0.94371799999999995</v>
+      </c>
+      <c r="S12" s="20">
+        <v>1.756033</v>
+      </c>
+      <c r="T12" s="43"/>
+      <c r="U12" s="24">
+        <v>229.29704899999999</v>
+      </c>
+      <c r="V12" s="24">
+        <f>U12/U7</f>
+        <v>1.5624410303794094</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="50"/>
       <c r="C13" s="20">
         <v>16</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="21">
         <v>0.37680000000000002</v>
       </c>
@@ -3296,584 +3449,586 @@
         <v>0.57709999999999995</v>
       </c>
       <c r="I13" s="20">
-        <v>0.62914599999999998</v>
+        <v>4.4219999999999997E-3</v>
       </c>
       <c r="J13" s="20">
-        <v>2.3740480000000002</v>
+        <f t="shared" si="0"/>
+        <v>226.14201718679331</v>
       </c>
       <c r="K13" s="20">
-        <v>4.4219999999999997E-3</v>
+        <f t="shared" si="1"/>
+        <v>904.56806874717324</v>
       </c>
       <c r="L13" s="20">
-        <v>853.33354193573803</v>
+        <v>0.45228299999999999</v>
       </c>
       <c r="M13" s="20">
-        <v>226.14155700000001</v>
-      </c>
-      <c r="N13" s="20">
-        <v>0.45228299999999999</v>
+        <f t="shared" si="2"/>
+        <v>2.1755880513733223</v>
       </c>
       <c r="O13" s="20">
-        <f t="shared" si="0"/>
-        <v>0.26500957232621009</v>
-      </c>
-      <c r="P13" s="20">
-        <f t="shared" si="1"/>
-        <v>2.1755880513733223</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="49">
-        <v>4</v>
-      </c>
-      <c r="C14" s="20">
-        <v>4</v>
-      </c>
-      <c r="D14" s="49">
-        <v>8192</v>
-      </c>
-      <c r="E14" s="49">
-        <v>150</v>
-      </c>
-      <c r="F14" s="21">
-        <v>7.0800000000000002E-2</v>
-      </c>
-      <c r="G14" s="21">
-        <v>1.5900000000000001E-2</v>
-      </c>
-      <c r="H14" s="21">
-        <v>8.5099999999999995E-2</v>
-      </c>
-      <c r="I14" s="20">
-        <v>5.0331599999999996</v>
-      </c>
-      <c r="J14" s="20">
-        <v>5.1649570000000002</v>
-      </c>
-      <c r="K14" s="20">
-        <v>9.6200000000000001E-3</v>
-      </c>
-      <c r="L14" s="20">
-        <v>106.667541935738</v>
-      </c>
-      <c r="M14" s="20">
-        <v>103.944895</v>
-      </c>
-      <c r="N14" s="20">
-        <v>0.20788999999999999</v>
-      </c>
+        <v>57344</v>
+      </c>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="20">
+        <v>469762048</v>
+      </c>
+      <c r="R13" s="20">
+        <v>1.101</v>
+      </c>
+      <c r="S13" s="20">
+        <v>1.9886269999999999</v>
+      </c>
+      <c r="T13" s="43"/>
+      <c r="U13" s="24">
+        <v>236.22431399999999</v>
+      </c>
+      <c r="V13" s="24">
+        <f>U13/U7</f>
+        <v>1.6096437445508911</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="53"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
       <c r="O14" s="20">
-        <f>M14/L14</f>
-        <v>0.97447539442337328</v>
-      </c>
-      <c r="P14" s="20">
-        <f>N14/N14</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="49"/>
-      <c r="C15" s="20">
-        <v>8</v>
-      </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="21">
-        <v>0.1137</v>
-      </c>
-      <c r="G15" s="21">
-        <v>3.1699999999999999E-2</v>
-      </c>
-      <c r="H15" s="21">
-        <v>0.15509999999999999</v>
-      </c>
-      <c r="I15" s="20">
-        <v>2.8311600000000001</v>
-      </c>
-      <c r="J15" s="20">
-        <v>3.0251169999999998</v>
-      </c>
-      <c r="K15" s="20">
-        <v>5.0090000000000004E-3</v>
-      </c>
-      <c r="L15" s="20">
-        <v>213.333541935738</v>
-      </c>
-      <c r="M15" s="20">
-        <v>199.65501399999999</v>
-      </c>
-      <c r="N15" s="20">
-        <v>0.39931</v>
-      </c>
-      <c r="O15" s="20">
-        <f t="shared" ref="O15:O20" si="2">M15/L15</f>
-        <v>0.93588196299736892</v>
-      </c>
-      <c r="P15" s="20">
-        <f>N15/$N$7</f>
-        <v>1.9207754100726346</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="49"/>
-      <c r="C16" s="20">
-        <v>16</v>
-      </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="21">
-        <v>0.20280000000000001</v>
-      </c>
-      <c r="G16" s="21">
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="H16" s="21">
-        <v>0.29420000000000002</v>
-      </c>
-      <c r="I16" s="20">
-        <v>0.15728600000000001</v>
-      </c>
-      <c r="J16" s="20">
-        <v>0.45901599999999998</v>
-      </c>
-      <c r="K16" s="20">
-        <v>6.8399999999999997E-3</v>
-      </c>
-      <c r="L16" s="20">
-        <v>426.66754193573797</v>
-      </c>
-      <c r="M16" s="20">
+        <v>65536</v>
+      </c>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="20">
+        <v>536870912</v>
+      </c>
+      <c r="R14" s="20">
+        <v>1.2582899999999999</v>
+      </c>
+      <c r="S14" s="20">
+        <v>2.1998060000000002</v>
+      </c>
+      <c r="T14" s="44"/>
+      <c r="U14" s="24">
         <v>244.053754</v>
       </c>
-      <c r="N16" s="20">
-        <v>0.48810799999999999</v>
-      </c>
-      <c r="O16" s="20">
-        <f t="shared" si="2"/>
-        <v>0.57199981253028587</v>
-      </c>
-      <c r="P16" s="20">
-        <f t="shared" ref="P16:P20" si="3">N16/$N$7</f>
-        <v>2.3479147626148444</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="49"/>
-      <c r="C17" s="20">
-        <v>32</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="21">
-        <v>0.37890000000000001</v>
-      </c>
-      <c r="G17" s="21">
-        <v>0.127</v>
-      </c>
-      <c r="H17" s="21">
-        <v>0.57330000000000003</v>
-      </c>
-      <c r="I17" s="20">
-        <v>0.55050200000000005</v>
-      </c>
-      <c r="J17" s="20">
-        <v>1.939594</v>
-      </c>
-      <c r="K17" s="20">
-        <v>4.8170000000000001E-3</v>
-      </c>
-      <c r="L17" s="20">
-        <v>853.33354193573803</v>
-      </c>
-      <c r="M17" s="20">
-        <v>207.596633</v>
-      </c>
-      <c r="N17" s="20">
-        <v>0.41519299999999998</v>
-      </c>
-      <c r="O17" s="20">
-        <f t="shared" si="2"/>
-        <v>0.24327724482630669</v>
-      </c>
-      <c r="P17" s="20">
-        <f t="shared" si="3"/>
-        <v>1.9971763913608158</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="49">
-        <v>8</v>
-      </c>
-      <c r="C18" s="20">
-        <v>4</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="21">
-        <v>0.1166</v>
-      </c>
-      <c r="G18" s="21">
-        <v>3.1699999999999999E-2</v>
-      </c>
-      <c r="H18" s="21">
-        <v>0.15840000000000001</v>
-      </c>
-      <c r="I18" s="20">
-        <v>2.8311600000000001</v>
-      </c>
-      <c r="J18" s="20">
-        <v>3.0313699999999999</v>
-      </c>
-      <c r="K18" s="20">
-        <v>5.019E-3</v>
-      </c>
-      <c r="L18" s="20">
-        <v>213.333541935738</v>
-      </c>
-      <c r="M18" s="20">
-        <v>199.24317300000001</v>
-      </c>
-      <c r="N18" s="20">
-        <v>0.39848600000000001</v>
-      </c>
-      <c r="O18" s="20">
-        <f t="shared" si="2"/>
-        <v>0.93395146019756048</v>
-      </c>
-      <c r="P18" s="20">
-        <f t="shared" si="3"/>
-        <v>1.916811775458175</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="49"/>
-      <c r="C19" s="20">
-        <v>8</v>
-      </c>
+      <c r="V14" s="24">
+        <f>U14/U7</f>
+        <v>1.66299392221015</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="53"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+    </row>
+    <row r="16" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="53"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="51">
+        <f>I22*8192*8192*10/1000000</f>
+        <v>2.7340151193600004</v>
+      </c>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+    </row>
+    <row r="17" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="53"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+    </row>
+    <row r="18" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="53"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
-      <c r="F19" s="21">
-        <v>0.2089</v>
-      </c>
-      <c r="G19" s="21">
-        <v>6.3500000000000001E-2</v>
-      </c>
-      <c r="H19" s="21">
-        <v>0.2979</v>
-      </c>
-      <c r="I19" s="20">
-        <v>1.4155800000000001</v>
-      </c>
-      <c r="J19" s="20">
-        <v>2.470313</v>
-      </c>
-      <c r="K19" s="20">
-        <v>4.0899999999999999E-3</v>
-      </c>
-      <c r="L19" s="20">
-        <v>426.66754193573797</v>
-      </c>
-      <c r="M19" s="20">
-        <v>244.49524299999999</v>
-      </c>
-      <c r="N19" s="20">
-        <v>0.48898999999999998</v>
-      </c>
-      <c r="O19" s="20">
-        <f t="shared" si="2"/>
-        <v>0.57303455025136252</v>
-      </c>
-      <c r="P19" s="20">
-        <f t="shared" si="3"/>
-        <v>2.3521573909278946</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="49"/>
-      <c r="C20" s="20">
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="B21" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="50">
+        <v>4</v>
+      </c>
+      <c r="C22" s="20">
+        <v>4</v>
+      </c>
+      <c r="D22" s="50">
+        <v>8192</v>
+      </c>
+      <c r="E22" s="38">
+        <v>100</v>
+      </c>
+      <c r="F22" s="21">
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="G22" s="21">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H22" s="21">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="I22" s="20">
+        <v>4.0740000000000004E-3</v>
+      </c>
+      <c r="J22" s="20">
+        <v>245.45</v>
+      </c>
+      <c r="K22" s="20">
+        <v>981.79</v>
+      </c>
+      <c r="L22" s="20">
+        <v>0.490896</v>
+      </c>
+      <c r="M22" s="20">
+        <f>L22/$L$22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="50"/>
+      <c r="C23" s="20">
+        <v>8</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="50"/>
+      <c r="C24" s="20">
         <v>16</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="21">
-        <v>0.37680000000000002</v>
-      </c>
-      <c r="G20" s="21">
-        <v>0.127</v>
-      </c>
-      <c r="H20" s="21">
-        <v>0.57709999999999995</v>
-      </c>
-      <c r="I20" s="20">
-        <v>0.62914599999999998</v>
-      </c>
-      <c r="J20" s="20">
-        <v>2.3740480000000002</v>
-      </c>
-      <c r="K20" s="20">
-        <v>4.4219999999999997E-3</v>
-      </c>
-      <c r="L20" s="20">
-        <v>853.33354193573803</v>
-      </c>
-      <c r="M20" s="20">
-        <v>226.14155700000001</v>
-      </c>
-      <c r="N20" s="20">
-        <v>0.45228299999999999</v>
-      </c>
-      <c r="O20" s="20">
-        <f t="shared" si="2"/>
-        <v>0.26500957232621009</v>
-      </c>
-      <c r="P20" s="20">
-        <f t="shared" si="3"/>
-        <v>2.1755880513733223</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="44" t="s">
+      <c r="D24" s="50"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="50"/>
+      <c r="C25" s="20">
+        <v>32</v>
+      </c>
+      <c r="D25" s="50"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="50">
+        <v>8</v>
+      </c>
+      <c r="C26" s="20">
+        <v>4</v>
+      </c>
+      <c r="D26" s="50"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="50"/>
+      <c r="C27" s="20">
+        <v>8</v>
+      </c>
+      <c r="D27" s="50"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="50"/>
+      <c r="C28" s="20">
+        <v>16</v>
+      </c>
+      <c r="D28" s="50"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="26"/>
+    </row>
+    <row r="32" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="B32" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="L32" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="20" t="s">
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" s="50">
+        <v>4</v>
+      </c>
+      <c r="C33" s="20">
+        <v>4</v>
+      </c>
+      <c r="D33" s="50">
+        <v>8192</v>
+      </c>
+      <c r="E33" s="38">
+        <v>200</v>
+      </c>
+      <c r="F33" s="21">
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="G33" s="21">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H33" s="21">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="I33" s="20">
+        <v>4.1770000000000002E-3</v>
+      </c>
+      <c r="J33" s="20">
+        <v>239.4</v>
+      </c>
+      <c r="K33" s="20">
+        <v>957.62</v>
+      </c>
+      <c r="L33" s="20">
+        <v>0.47880800000000001</v>
+      </c>
+      <c r="M33" s="20">
+        <f>L33/$L$33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" s="50"/>
+      <c r="C34" s="20">
+        <v>8</v>
+      </c>
+      <c r="D34" s="50"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="50"/>
+      <c r="C35" s="20">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="20">
-        <v>8192</v>
-      </c>
-      <c r="C25" s="38">
-        <v>8192</v>
-      </c>
-      <c r="D25" s="20">
-        <v>67108864</v>
-      </c>
-      <c r="E25" s="20">
-        <v>0.15728600000000001</v>
-      </c>
-      <c r="F25" s="20">
-        <v>0.457283</v>
-      </c>
-      <c r="G25" s="41">
-        <v>426.66754193573797</v>
-      </c>
-      <c r="H25" s="25">
-        <v>146.75565</v>
-      </c>
-      <c r="I25" s="25">
-        <f>H25/H25</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="20">
-        <v>16384</v>
-      </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="20">
-        <v>134217728</v>
-      </c>
-      <c r="E26" s="20">
-        <v>0.31457299999999999</v>
-      </c>
-      <c r="F26" s="20">
-        <v>0.72777099999999995</v>
-      </c>
-      <c r="G26" s="42"/>
-      <c r="H26" s="25">
-        <v>184.423023</v>
-      </c>
-      <c r="I26" s="25">
-        <f>H26/H25</f>
-        <v>1.2566672765239362</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="20">
-        <v>24576</v>
-      </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="20">
-        <v>201326592</v>
-      </c>
-      <c r="E27" s="20">
-        <v>0.47185899999999997</v>
-      </c>
-      <c r="F27" s="20">
-        <v>0.99838400000000005</v>
-      </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="25">
-        <v>201.65246200000001</v>
-      </c>
-      <c r="I27" s="25">
-        <f>H27/H25</f>
-        <v>1.3740694957911332</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="20">
-        <v>32768</v>
-      </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="20">
-        <v>268435456</v>
-      </c>
-      <c r="E28" s="20">
-        <v>0.62914599999999998</v>
-      </c>
-      <c r="F28" s="20">
-        <v>1.2690570000000001</v>
-      </c>
-      <c r="G28" s="42"/>
-      <c r="H28" s="25">
-        <v>211.523561</v>
-      </c>
-      <c r="I28" s="25">
-        <f>H28/H25</f>
-        <v>1.4413316352726453</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="20">
-        <v>40960</v>
-      </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="20">
-        <v>335544320</v>
-      </c>
-      <c r="E29" s="20">
-        <v>0.78643200000000002</v>
-      </c>
-      <c r="F29" s="20">
-        <v>1.5138590000000001</v>
-      </c>
-      <c r="G29" s="42"/>
-      <c r="H29" s="25">
-        <v>221.64833100000001</v>
-      </c>
-      <c r="I29" s="25">
-        <f>H29/H25</f>
-        <v>1.5103223010493976</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="20">
-        <v>49152</v>
-      </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="20">
-        <v>402653184</v>
-      </c>
-      <c r="E30" s="20">
-        <v>0.94371799999999995</v>
-      </c>
-      <c r="F30" s="20">
-        <v>1.756033</v>
-      </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="25">
-        <v>229.29704899999999</v>
-      </c>
-      <c r="I30" s="25">
-        <f>H30/H25</f>
-        <v>1.5624410303794094</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="20">
-        <v>57344</v>
-      </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="20">
-        <v>469762048</v>
-      </c>
-      <c r="E31" s="20">
-        <v>1.101</v>
-      </c>
-      <c r="F31" s="20">
-        <v>1.9886269999999999</v>
-      </c>
-      <c r="G31" s="42"/>
-      <c r="H31" s="25">
-        <v>236.22431399999999</v>
-      </c>
-      <c r="I31" s="25">
-        <f>H31/H25</f>
-        <v>1.6096437445508911</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="20">
-        <v>65536</v>
-      </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="20">
-        <v>536870912</v>
-      </c>
-      <c r="E32" s="20">
-        <v>1.2582899999999999</v>
-      </c>
-      <c r="F32" s="20">
-        <v>2.1998060000000002</v>
-      </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="25">
-        <v>244.053754</v>
-      </c>
-      <c r="I32" s="25">
-        <f>H32/H25</f>
-        <v>1.66299392221015</v>
-      </c>
+      <c r="D35" s="50"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" s="50"/>
+      <c r="C36" s="20">
+        <v>32</v>
+      </c>
+      <c r="D36" s="50"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="50">
+        <v>8</v>
+      </c>
+      <c r="C37" s="20">
+        <v>4</v>
+      </c>
+      <c r="D37" s="50"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38" s="50"/>
+      <c r="C38" s="20">
+        <v>8</v>
+      </c>
+      <c r="D38" s="50"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" s="50"/>
+      <c r="C39" s="20">
+        <v>16</v>
+      </c>
+      <c r="D39" s="50"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="C25:C32"/>
-    <mergeCell ref="G25:G32"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="O5:P5"/>
+  <mergeCells count="27">
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="D33:D39"/>
+    <mergeCell ref="E33:E39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="P7:P14"/>
+    <mergeCell ref="T7:T14"/>
+    <mergeCell ref="O5:V5"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="D7:D13"/>
     <mergeCell ref="E7:E13"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="D14:D20"/>
-    <mergeCell ref="E14:E20"/>
-    <mergeCell ref="B18:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated with the freq=100 c-slowing data
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Coding/Research/ImperialSummerReports/assets/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" activeTab="2"/>
+    <workbookView xWindow="1065" yWindow="465" windowWidth="27735" windowHeight="17535" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
     <sheet name="Standard CSRp" sheetId="2" r:id="rId2"/>
     <sheet name="BCSR" sheetId="3" r:id="rId3"/>
+    <sheet name="study of data size and speed" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>numPipes</t>
   </si>
@@ -211,6 +207,33 @@
         <rFont val="Consolas"/>
       </rPr>
       <t xml:space="preserve"> C-Slowing(L=16)</t>
+    </r>
+  </si>
+  <si>
+    <t>Time per
+element
+(us)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Experiment data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>w/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> C-Slowing(L=16, Freq=100)</t>
     </r>
   </si>
 </sst>
@@ -455,6 +478,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,7 +518,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -518,21 +556,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -704,40 +727,40 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>BCSR!$O$7:$O$14</c:f>
+              <c:f>'study of data size and speed'!$C$5:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8192.0</c:v>
+                  <c:v>8192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16384.0</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24576.0</c:v>
+                  <c:v>24576</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32768.0</c:v>
+                  <c:v>32768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40960.0</c:v>
+                  <c:v>40960</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49152.0</c:v>
+                  <c:v>49152</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57344.0</c:v>
+                  <c:v>57344</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>65536.0</c:v>
+                  <c:v>65536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BCSR!$U$7:$U$14</c:f>
+              <c:f>'study of data size and speed'!$I$5:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -748,19 +771,19 @@
                   <c:v>184.423023</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201.652462</c:v>
+                  <c:v>201.65246200000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>211.523561</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>221.648331</c:v>
+                  <c:v>221.64833100000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>229.297049</c:v>
+                  <c:v>229.29704899999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>236.224314</c:v>
+                  <c:v>236.22431399999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>244.053754</c:v>
@@ -780,11 +803,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2120314704"/>
-        <c:axId val="-2131183280"/>
+        <c:axId val="415624632"/>
+        <c:axId val="415623456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120314704"/>
+        <c:axId val="415624632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,7 +916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131183280"/>
+        <c:crossAx val="415623456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -901,7 +924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131183280"/>
+        <c:axId val="415623456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -999,7 +1022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120314704"/>
+        <c:crossAx val="415624632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1615,20 +1638,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>458611</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>117592</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>431330</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>94543</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>429919</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>167451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1941,36 +1964,36 @@
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="N2" s="29" t="s">
+      <c r="H2" s="31"/>
+      <c r="N2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2017,11 +2040,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="32">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -2042,10 +2065,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="34">
         <v>8192</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="34">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -2065,9 +2088,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -2086,8 +2109,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -2105,9 +2128,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -2126,8 +2149,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -2145,9 +2168,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -2166,8 +2189,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30">
+      <c r="N7" s="34"/>
+      <c r="O7" s="34">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -2187,9 +2210,9 @@
         <v>1.6368964094098226</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -2207,9 +2230,9 @@
         <v>1.9411943936624008</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -2227,9 +2250,9 @@
         <v>1.9749886655584104</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N10" s="30"/>
-      <c r="O10" s="30">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N10" s="34"/>
+      <c r="O10" s="34">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -2249,9 +2272,9 @@
         <v>1.8745356995460174</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -2269,9 +2292,9 @@
         <v>3.5057129798903106</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -2289,9 +2312,9 @@
         <v>3.8351972192836636</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N13" s="30"/>
-      <c r="O13" s="30">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N13" s="34"/>
+      <c r="O13" s="34">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -2311,9 +2334,9 @@
         <v>1.3601320676846882</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -2331,9 +2354,9 @@
         <v>5.157678244972578</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -2351,7 +2374,7 @@
         <v>7.2476953302100657</v>
       </c>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="2"/>
     </row>
   </sheetData>
@@ -2380,82 +2403,82 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11.83203125" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="35" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="35" t="s">
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="37"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="41"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="29"/>
+      <c r="I4" s="33"/>
       <c r="J4" s="2"/>
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="34" t="s">
+      <c r="L4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="29"/>
+      <c r="M4" s="33"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="29"/>
+      <c r="Q4" s="33"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2505,8 +2528,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="30">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
         <v>8192</v>
       </c>
       <c r="B6" s="6">
@@ -2561,8 +2584,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -2618,8 +2641,8 @@
         <v>1.961091731513781</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -2675,8 +2698,8 @@
         <v>3.7350787748687084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -2732,8 +2755,8 @@
         <v>6.4978725035458273</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
       <c r="B10" s="7">
         <v>16</v>
       </c>
@@ -2789,8 +2812,8 @@
         <v>9.8531069114884815</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
       <c r="B11" s="7">
         <v>32</v>
       </c>
@@ -2846,8 +2869,8 @@
         <v>8.088166519722467</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
       <c r="B12" s="7">
         <v>64</v>
       </c>
@@ -2860,24 +2883,24 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="33"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="37"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
       <c r="B13" s="7">
         <v>128</v>
       </c>
@@ -2904,8 +2927,8 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="30"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
       <c r="B14" s="7">
         <v>256</v>
       </c>
@@ -2932,7 +2955,7 @@
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24">
         <f>I8/BCSR!L9</f>
         <v>0.20105386512820933</v>
@@ -2960,69 +2983,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:V39"/>
+  <dimension ref="B4:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="108" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
     <col min="9" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="49" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-    </row>
-    <row r="5" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="48" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+    </row>
+    <row r="5" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
       <c r="M5" s="26"/>
-      <c r="O5" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="47"/>
-    </row>
-    <row r="6" spans="2:22" s="18" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:13" s="18" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
         <v>29</v>
       </c>
@@ -3059,42 +3073,18 @@
       <c r="M6" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="V6" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="50">
+    </row>
+    <row r="7" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44">
         <v>4</v>
       </c>
       <c r="C7" s="20">
         <v>4</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="44">
         <v>8192</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="44">
         <v>100</v>
       </c>
       <c r="F7" s="21">
@@ -3124,39 +3114,14 @@
         <f>L7/L7</f>
         <v>1</v>
       </c>
-      <c r="O7" s="20">
-        <v>8192</v>
-      </c>
-      <c r="P7" s="39">
-        <v>8192</v>
-      </c>
-      <c r="Q7" s="20">
-        <v>67108864</v>
-      </c>
-      <c r="R7" s="20">
-        <v>0.15728600000000001</v>
-      </c>
-      <c r="S7" s="20">
-        <v>0.457283</v>
-      </c>
-      <c r="T7" s="42">
-        <v>426.66754193573797</v>
-      </c>
-      <c r="U7" s="24">
-        <v>146.75565</v>
-      </c>
-      <c r="V7" s="24">
-        <f>U7/U7</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="50"/>
+    </row>
+    <row r="8" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
       <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="21">
         <v>0.1137</v>
       </c>
@@ -3174,7 +3139,7 @@
         <v>199.64064683569572</v>
       </c>
       <c r="K8" s="20">
-        <f t="shared" ref="K8:K13" si="1">4/I8</f>
+        <f>4/I8</f>
         <v>798.56258734278288</v>
       </c>
       <c r="L8" s="20">
@@ -3184,35 +3149,14 @@
         <f>L8/$L$7</f>
         <v>1.9207754100726346</v>
       </c>
-      <c r="O8" s="20">
-        <v>16384</v>
-      </c>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="20">
-        <v>134217728</v>
-      </c>
-      <c r="R8" s="20">
-        <v>0.31457299999999999</v>
-      </c>
-      <c r="S8" s="20">
-        <v>0.72777099999999995</v>
-      </c>
-      <c r="T8" s="43"/>
-      <c r="U8" s="24">
-        <v>184.423023</v>
-      </c>
-      <c r="V8" s="24">
-        <f>U8/U7</f>
-        <v>1.2566672765239362</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="50"/>
+    </row>
+    <row r="9" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
       <c r="C9" s="20">
         <v>16</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="21">
         <v>0.20280000000000001</v>
       </c>
@@ -3230,45 +3174,24 @@
         <v>146.19883040935673</v>
       </c>
       <c r="K9" s="20">
-        <f t="shared" si="1"/>
+        <f>4/I9</f>
         <v>584.79532163742692</v>
       </c>
       <c r="L9" s="20">
         <v>0.48810799999999999</v>
       </c>
       <c r="M9" s="20">
-        <f t="shared" ref="M9:M13" si="2">L9/$L$7</f>
+        <f t="shared" ref="M9:M13" si="1">L9/$L$7</f>
         <v>2.3479147626148444</v>
       </c>
-      <c r="O9" s="20">
-        <v>24576</v>
-      </c>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="20">
-        <v>201326592</v>
-      </c>
-      <c r="R9" s="20">
-        <v>0.47185899999999997</v>
-      </c>
-      <c r="S9" s="20">
-        <v>0.99838400000000005</v>
-      </c>
-      <c r="T9" s="43"/>
-      <c r="U9" s="24">
-        <v>201.65246200000001</v>
-      </c>
-      <c r="V9" s="24">
-        <f>U9/U7</f>
-        <v>1.3740694957911332</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="50"/>
+    </row>
+    <row r="10" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
       <c r="C10" s="20">
         <v>32</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="21">
         <v>0.37890000000000001</v>
       </c>
@@ -3286,47 +3209,26 @@
         <v>207.59809009757109</v>
       </c>
       <c r="K10" s="20">
-        <f t="shared" si="1"/>
+        <f>4/I10</f>
         <v>830.39236039028435</v>
       </c>
       <c r="L10" s="20">
         <v>0.41519299999999998</v>
       </c>
       <c r="M10" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9971763913608158</v>
       </c>
-      <c r="O10" s="20">
-        <v>32768</v>
-      </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="20">
-        <v>268435456</v>
-      </c>
-      <c r="R10" s="20">
-        <v>0.62914599999999998</v>
-      </c>
-      <c r="S10" s="20">
-        <v>1.2690570000000001</v>
-      </c>
-      <c r="T10" s="43"/>
-      <c r="U10" s="24">
-        <v>211.523561</v>
-      </c>
-      <c r="V10" s="24">
-        <f>U10/U7</f>
-        <v>1.4413316352726453</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="50">
+    </row>
+    <row r="11" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="44">
         <v>8</v>
       </c>
       <c r="C11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="21">
         <v>0.1166</v>
       </c>
@@ -3344,45 +3246,24 @@
         <v>199.24287706714486</v>
       </c>
       <c r="K11" s="20">
-        <f t="shared" si="1"/>
+        <f>4/I11</f>
         <v>796.97150826857944</v>
       </c>
       <c r="L11" s="20">
         <v>0.39848600000000001</v>
       </c>
       <c r="M11" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.916811775458175</v>
       </c>
-      <c r="O11" s="20">
-        <v>40960</v>
-      </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="20">
-        <v>335544320</v>
-      </c>
-      <c r="R11" s="20">
-        <v>0.78643200000000002</v>
-      </c>
-      <c r="S11" s="20">
-        <v>1.5138590000000001</v>
-      </c>
-      <c r="T11" s="43"/>
-      <c r="U11" s="24">
-        <v>221.64833100000001</v>
-      </c>
-      <c r="V11" s="24">
-        <f>U11/U7</f>
-        <v>1.5103223010493976</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="50"/>
+    </row>
+    <row r="12" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
       <c r="C12" s="20">
         <v>8</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="21">
         <v>0.2089</v>
       </c>
@@ -3400,45 +3281,24 @@
         <v>244.49877750611248</v>
       </c>
       <c r="K12" s="20">
-        <f t="shared" si="1"/>
+        <f>4/I12</f>
         <v>977.9951100244499</v>
       </c>
       <c r="L12" s="20">
         <v>0.48898999999999998</v>
       </c>
       <c r="M12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.3521573909278946</v>
       </c>
-      <c r="O12" s="20">
-        <v>49152</v>
-      </c>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="20">
-        <v>402653184</v>
-      </c>
-      <c r="R12" s="20">
-        <v>0.94371799999999995</v>
-      </c>
-      <c r="S12" s="20">
-        <v>1.756033</v>
-      </c>
-      <c r="T12" s="43"/>
-      <c r="U12" s="24">
-        <v>229.29704899999999</v>
-      </c>
-      <c r="V12" s="24">
-        <f>U12/U7</f>
-        <v>1.5624410303794094</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="50"/>
+    </row>
+    <row r="13" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="44"/>
       <c r="C13" s="20">
         <v>16</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="21">
         <v>0.37680000000000002</v>
       </c>
@@ -3456,167 +3316,122 @@
         <v>226.14201718679331</v>
       </c>
       <c r="K13" s="20">
-        <f t="shared" si="1"/>
+        <f>4/I13</f>
         <v>904.56806874717324</v>
       </c>
       <c r="L13" s="20">
         <v>0.45228299999999999</v>
       </c>
       <c r="M13" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.1755880513733223</v>
       </c>
-      <c r="O13" s="20">
-        <v>57344</v>
-      </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="20">
-        <v>469762048</v>
-      </c>
-      <c r="R13" s="20">
-        <v>1.101</v>
-      </c>
-      <c r="S13" s="20">
-        <v>1.9886269999999999</v>
-      </c>
-      <c r="T13" s="43"/>
-      <c r="U13" s="24">
-        <v>236.22431399999999</v>
-      </c>
-      <c r="V13" s="24">
-        <f>U13/U7</f>
-        <v>1.6096437445508911</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="53"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="O14" s="20">
-        <v>65536</v>
-      </c>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="20">
-        <v>536870912</v>
-      </c>
-      <c r="R14" s="20">
-        <v>1.2582899999999999</v>
-      </c>
-      <c r="S14" s="20">
-        <v>2.1998060000000002</v>
-      </c>
-      <c r="T14" s="44"/>
-      <c r="U14" s="24">
-        <v>244.053754</v>
-      </c>
-      <c r="V14" s="24">
-        <f>U14/U7</f>
-        <v>1.66299392221015</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="53"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-    </row>
-    <row r="16" spans="2:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="53"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="51">
-        <f>I22*8192*8192*10/1000000</f>
-        <v>2.7340151193600004</v>
-      </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-    </row>
-    <row r="17" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="53"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-    </row>
-    <row r="18" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="53"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="48" t="s">
+    </row>
+    <row r="14" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="29"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="29"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="29"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48" t="s">
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>29</v>
       </c>
@@ -3639,7 +3454,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J21" s="22" t="s">
         <v>44</v>
@@ -3654,17 +3469,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="50">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="44">
         <v>4</v>
       </c>
       <c r="C22" s="20">
         <v>4</v>
       </c>
-      <c r="D22" s="50">
+      <c r="D22" s="44">
         <v>8192</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="43">
         <v>100</v>
       </c>
       <c r="F22" s="21">
@@ -3677,361 +3492,706 @@
         <v>8.4599999999999995E-2</v>
       </c>
       <c r="I22" s="20">
-        <v>4.0740000000000004E-3</v>
+        <v>4.9699999999999996E-3</v>
       </c>
       <c r="J22" s="20">
-        <v>245.45</v>
+        <v>12.58</v>
       </c>
       <c r="K22" s="20">
-        <v>981.79</v>
+        <v>804.89</v>
       </c>
       <c r="L22" s="20">
-        <v>0.490896</v>
+        <v>0.402443</v>
       </c>
       <c r="M22" s="20">
         <f>L22/$L$22</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="50"/>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="44"/>
       <c r="C23" s="20">
         <v>8</v>
       </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B24" s="50"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="21">
+        <v>0.11</v>
+      </c>
+      <c r="G23" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H23" s="21">
+        <v>0.15409999999999999</v>
+      </c>
+      <c r="I23" s="20">
+        <v>5.7029999999999997E-3</v>
+      </c>
+      <c r="J23">
+        <v>5.48</v>
+      </c>
+      <c r="K23" s="20">
+        <v>701.36</v>
+      </c>
+      <c r="L23" s="20">
+        <v>0.35068199999999999</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" ref="M23:M28" si="2">L23/$L$22</f>
+        <v>0.87138302815554003</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="44"/>
       <c r="C24" s="20">
         <v>16</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="50"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="21">
+        <v>0.2036</v>
+      </c>
+      <c r="G24" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H24" s="21">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="I24" s="20">
+        <v>6.7140000000000003E-3</v>
+      </c>
+      <c r="J24" s="20">
+        <v>2.33</v>
+      </c>
+      <c r="K24" s="20">
+        <v>595.79</v>
+      </c>
+      <c r="L24" s="20">
+        <v>0.29789300000000002</v>
+      </c>
+      <c r="M24" s="20">
+        <f t="shared" si="2"/>
+        <v>0.74021165730302185</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="44"/>
       <c r="C25" s="20">
         <v>32</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="50">
+      <c r="D25" s="44"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="21">
+        <v>0.37430000000000002</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0.127</v>
+      </c>
+      <c r="H25" s="21">
+        <v>0.57240000000000002</v>
+      </c>
+      <c r="I25" s="20">
+        <v>9.3740000000000004E-3</v>
+      </c>
+      <c r="J25" s="20">
+        <v>0.83</v>
+      </c>
+      <c r="K25" s="20">
+        <v>426.73</v>
+      </c>
+      <c r="L25" s="20">
+        <v>0.213365</v>
+      </c>
+      <c r="M25" s="20">
+        <f t="shared" si="2"/>
+        <v>0.53017445948867292</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="44">
         <v>8</v>
       </c>
       <c r="C26" s="20">
         <v>4</v>
       </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="50"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="21">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G26" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H26" s="21">
+        <v>0.15790000000000001</v>
+      </c>
+      <c r="I26" s="20">
+        <v>5.5710000000000004E-3</v>
+      </c>
+      <c r="J26" s="20">
+        <v>5.61</v>
+      </c>
+      <c r="K26" s="20">
+        <v>717.98</v>
+      </c>
+      <c r="L26" s="20">
+        <v>0.358991</v>
+      </c>
+      <c r="M26" s="20">
+        <f t="shared" si="2"/>
+        <v>0.89202943025471937</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="44"/>
       <c r="C27" s="20">
         <v>8</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="50"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="21">
+        <v>0.2046</v>
+      </c>
+      <c r="G27" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H27" s="21">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="I27" s="20">
+        <v>6.7279999999999996E-3</v>
+      </c>
+      <c r="J27" s="20">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="K27" s="20">
+        <v>594.57000000000005</v>
+      </c>
+      <c r="L27" s="20">
+        <v>0.29728599999999999</v>
+      </c>
+      <c r="M27" s="20">
+        <f t="shared" si="2"/>
+        <v>0.73870336917277724</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="44"/>
       <c r="C28" s="20">
         <v>16</v>
       </c>
-      <c r="D28" s="50"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="49" t="s">
+      <c r="D28" s="44"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="21">
+        <v>0.38140000000000002</v>
+      </c>
+      <c r="G28" s="21">
+        <v>0.127</v>
+      </c>
+      <c r="H28" s="21">
+        <v>0.57609999999999995</v>
+      </c>
+      <c r="I28" s="20">
+        <v>9.4280000000000006E-3</v>
+      </c>
+      <c r="J28" s="20">
+        <v>0.83</v>
+      </c>
+      <c r="K28" s="20">
+        <v>424.28</v>
+      </c>
+      <c r="L28" s="20">
+        <v>0.21214</v>
+      </c>
+      <c r="M28" s="20">
+        <f t="shared" si="2"/>
+        <v>0.52713055016486809</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B31" s="48" t="s">
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="45"/>
+      <c r="M43" s="45"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48" t="s">
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="26"/>
-    </row>
-    <row r="32" spans="2:13" ht="45" x14ac:dyDescent="0.2">
-      <c r="B32" s="25" t="s">
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="M44" s="26"/>
+    </row>
+    <row r="45" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C45" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D45" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E45" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="F45" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="25" t="s">
+      <c r="G45" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="25" t="s">
+      <c r="H45" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="22" t="s">
+      <c r="I45" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J32" s="22" t="s">
+      <c r="J45" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="K32" s="22" t="s">
+      <c r="K45" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="L32" s="25" t="s">
+      <c r="L45" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M32" s="25" t="s">
+      <c r="M45" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B33" s="50">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="44">
         <v>4</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C46" s="20">
         <v>4</v>
       </c>
-      <c r="D33" s="50">
+      <c r="D46" s="44">
         <v>8192</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E46" s="43">
         <v>200</v>
       </c>
-      <c r="F33" s="21">
+      <c r="F46" s="21">
         <v>5.9700000000000003E-2</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G46" s="21">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="H33" s="21">
+      <c r="H46" s="21">
         <v>8.4599999999999995E-2</v>
       </c>
-      <c r="I33" s="20">
+      <c r="I46" s="20">
         <v>4.1770000000000002E-3</v>
       </c>
-      <c r="J33" s="20">
+      <c r="J46" s="20">
         <v>239.4</v>
       </c>
-      <c r="K33" s="20">
+      <c r="K46" s="20">
         <v>957.62</v>
       </c>
-      <c r="L33" s="20">
+      <c r="L46" s="20">
         <v>0.47880800000000001</v>
       </c>
-      <c r="M33" s="20">
-        <f>L33/$L$33</f>
+      <c r="M46" s="20">
+        <f>L46/$L$46</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="50"/>
-      <c r="C34" s="20">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="44"/>
+      <c r="C47" s="20">
         <v>8</v>
       </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B35" s="50"/>
-      <c r="C35" s="20">
+      <c r="D47" s="44"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="44"/>
+      <c r="C48" s="20">
         <v>16</v>
       </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B36" s="50"/>
-      <c r="C36" s="20">
+      <c r="D48" s="44"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="44"/>
+      <c r="C49" s="20">
         <v>32</v>
       </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B37" s="50">
+      <c r="D49" s="44"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="44">
         <v>8</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C50" s="20">
         <v>4</v>
       </c>
-      <c r="D37" s="50"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="50"/>
-      <c r="C38" s="20">
+      <c r="D50" s="44"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="44"/>
+      <c r="C51" s="20">
         <v>8</v>
       </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B39" s="50"/>
-      <c r="C39" s="20">
+      <c r="D51" s="44"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="44"/>
+      <c r="C52" s="20">
         <v>16</v>
       </c>
-      <c r="D39" s="50"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="D33:D39"/>
-    <mergeCell ref="E33:E39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B30:M30"/>
+  <mergeCells count="24">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="E7:E13"/>
+    <mergeCell ref="F5:H5"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:L20"/>
     <mergeCell ref="I5:L5"/>
-    <mergeCell ref="P7:P14"/>
-    <mergeCell ref="T7:T14"/>
-    <mergeCell ref="O5:V5"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="D7:D13"/>
-    <mergeCell ref="E7:E13"/>
-    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B43:M43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="E46:E52"/>
+    <mergeCell ref="B50:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:J12"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="20">
+        <v>8192</v>
+      </c>
+      <c r="D5" s="46">
+        <v>8192</v>
+      </c>
+      <c r="E5" s="20">
+        <v>67108864</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.15728600000000001</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0.457283</v>
+      </c>
+      <c r="H5" s="49">
+        <v>426.66754193573797</v>
+      </c>
+      <c r="I5" s="24">
+        <v>146.75565</v>
+      </c>
+      <c r="J5" s="24">
+        <f>I5/I5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="20">
+        <v>16384</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="20">
+        <v>134217728</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0.31457299999999999</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0.72777099999999995</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="24">
+        <v>184.423023</v>
+      </c>
+      <c r="J6" s="24">
+        <f>I6/I5</f>
+        <v>1.2566672765239362</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="20">
+        <v>24576</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="20">
+        <v>201326592</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0.47185899999999997</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0.99838400000000005</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="24">
+        <v>201.65246200000001</v>
+      </c>
+      <c r="J7" s="24">
+        <f>I7/I5</f>
+        <v>1.3740694957911332</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="20">
+        <v>32768</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="20">
+        <v>268435456</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0.62914599999999998</v>
+      </c>
+      <c r="G8" s="20">
+        <v>1.2690570000000001</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="24">
+        <v>211.523561</v>
+      </c>
+      <c r="J8" s="24">
+        <f>I8/I5</f>
+        <v>1.4413316352726453</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="20">
+        <v>40960</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="20">
+        <v>335544320</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0.78643200000000002</v>
+      </c>
+      <c r="G9" s="20">
+        <v>1.5138590000000001</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" s="24">
+        <v>221.64833100000001</v>
+      </c>
+      <c r="J9" s="24">
+        <f>I9/I5</f>
+        <v>1.5103223010493976</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="20">
+        <v>49152</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="20">
+        <v>402653184</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.94371799999999995</v>
+      </c>
+      <c r="G10" s="20">
+        <v>1.756033</v>
+      </c>
+      <c r="H10" s="50"/>
+      <c r="I10" s="24">
+        <v>229.29704899999999</v>
+      </c>
+      <c r="J10" s="24">
+        <f>I10/I5</f>
+        <v>1.5624410303794094</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="20">
+        <v>57344</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="20">
+        <v>469762048</v>
+      </c>
+      <c r="F11" s="20">
+        <v>1.101</v>
+      </c>
+      <c r="G11" s="20">
+        <v>1.9886269999999999</v>
+      </c>
+      <c r="H11" s="50"/>
+      <c r="I11" s="24">
+        <v>236.22431399999999</v>
+      </c>
+      <c r="J11" s="24">
+        <f>I11/I5</f>
+        <v>1.6096437445508911</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="20">
+        <v>65536</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="20">
+        <v>536870912</v>
+      </c>
+      <c r="F12" s="20">
+        <v>1.2582899999999999</v>
+      </c>
+      <c r="G12" s="20">
+        <v>2.1998060000000002</v>
+      </c>
+      <c r="H12" s="51"/>
+      <c r="I12" s="24">
+        <v>244.053754</v>
+      </c>
+      <c r="J12" s="24">
+        <f>I12/I5</f>
+        <v>1.66299392221015</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="H5:H12"/>
+    <mergeCell ref="C3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated with new 200MHz data
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="465" windowWidth="27735" windowHeight="17535" activeTab="2"/>
+    <workbookView xWindow="1065" yWindow="465" windowWidth="27735" windowHeight="17535" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CSRp" sheetId="1" r:id="rId1"/>
     <sheet name="Standard CSRp" sheetId="2" r:id="rId2"/>
-    <sheet name="BCSR" sheetId="3" r:id="rId3"/>
-    <sheet name="study of data size and speed" sheetId="4" r:id="rId4"/>
+    <sheet name="BCSR no ROM opt" sheetId="3" r:id="rId3"/>
+    <sheet name="BCSR ROM opt." sheetId="5" r:id="rId4"/>
+    <sheet name="study of data size and speed" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
   <si>
     <t>numPipes</t>
   </si>
@@ -235,6 +236,35 @@
       </rPr>
       <t xml:space="preserve"> C-Slowing(L=16, Freq=100)</t>
     </r>
+  </si>
+  <si>
+    <t>ROM
+size</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Experiment data </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>w/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> C-Slowing(L=16, Freq=200)</t>
+    </r>
+  </si>
+  <si>
+    <t>FAILED TIMING</t>
   </si>
 </sst>
 </file>
@@ -416,7 +446,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -484,6 +514,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,14 +556,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,6 +590,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -618,7 +663,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -706,7 +750,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -803,11 +846,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="415624632"/>
-        <c:axId val="415623456"/>
+        <c:axId val="166716608"/>
+        <c:axId val="166717392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="415624632"/>
+        <c:axId val="166716608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +898,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -916,7 +958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415623456"/>
+        <c:crossAx val="166717392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -924,7 +966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="415623456"/>
+        <c:axId val="166717392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +1009,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1022,7 +1063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415624632"/>
+        <c:crossAx val="166716608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1974,23 +2015,23 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="N2" s="33" t="s">
+      <c r="H2" s="33"/>
+      <c r="N2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2041,10 +2082,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="34">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -2065,10 +2106,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="34">
+      <c r="N4" s="36">
         <v>8192</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="36">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -2089,8 +2130,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -2109,8 +2150,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -2129,8 +2170,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -2149,8 +2190,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -2169,8 +2210,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -2189,8 +2230,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34">
+      <c r="N7" s="36"/>
+      <c r="O7" s="36">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -2211,8 +2252,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -2231,8 +2272,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -2251,8 +2292,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="34"/>
-      <c r="O10" s="34">
+      <c r="N10" s="36"/>
+      <c r="O10" s="36">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -2273,8 +2314,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -2293,8 +2334,8 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -2313,8 +2354,8 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N13" s="34"/>
-      <c r="O13" s="34">
+      <c r="N13" s="36"/>
+      <c r="O13" s="36">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -2335,8 +2376,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -2355,8 +2396,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -2413,72 +2454,72 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="39" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="39" t="s">
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="41"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="43"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="33"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="2"/>
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="33"/>
+      <c r="M4" s="35"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="P4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="33"/>
+      <c r="Q4" s="35"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2529,7 +2570,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="36">
         <v>8192</v>
       </c>
       <c r="B6" s="6">
@@ -2585,7 +2626,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -2642,7 +2683,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -2699,7 +2740,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -2756,7 +2797,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="7">
         <v>16</v>
       </c>
@@ -2813,7 +2854,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="7">
         <v>32</v>
       </c>
@@ -2870,7 +2911,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="7">
         <v>64</v>
       </c>
@@ -2883,24 +2924,24 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="39"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="7">
         <v>128</v>
       </c>
@@ -2928,7 +2969,7 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="7">
         <v>256</v>
       </c>
@@ -2957,7 +2998,7 @@
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24">
-        <f>I8/BCSR!L9</f>
+        <f>I8/'BCSR no ROM opt'!L9</f>
         <v>0.20105386512820933</v>
       </c>
     </row>
@@ -2985,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:M19"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,37 +3044,37 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
     </row>
     <row r="5" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
       <c r="M5" s="26"/>
     </row>
     <row r="6" spans="2:13" s="18" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3075,16 +3116,16 @@
       </c>
     </row>
     <row r="7" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="44">
+      <c r="B7" s="45">
         <v>4</v>
       </c>
       <c r="C7" s="20">
         <v>4</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="45">
         <v>8192</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="45">
         <v>100</v>
       </c>
       <c r="F7" s="21">
@@ -3104,7 +3145,7 @@
         <v>103.95010395010395</v>
       </c>
       <c r="K7" s="20">
-        <f>4/I7</f>
+        <f t="shared" ref="K7:K13" si="0">4/I7</f>
         <v>415.80041580041581</v>
       </c>
       <c r="L7" s="20">
@@ -3116,12 +3157,12 @@
       </c>
     </row>
     <row r="8" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="21">
         <v>0.1137</v>
       </c>
@@ -3135,11 +3176,11 @@
         <v>5.0090000000000004E-3</v>
       </c>
       <c r="J8" s="20">
-        <f t="shared" ref="J8:J13" si="0">1/I8</f>
+        <f t="shared" ref="J8:J13" si="1">1/I8</f>
         <v>199.64064683569572</v>
       </c>
       <c r="K8" s="20">
-        <f>4/I8</f>
+        <f t="shared" si="0"/>
         <v>798.56258734278288</v>
       </c>
       <c r="L8" s="20">
@@ -3151,12 +3192,12 @@
       </c>
     </row>
     <row r="9" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="20">
         <v>16</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="21">
         <v>0.20280000000000001</v>
       </c>
@@ -3170,28 +3211,28 @@
         <v>6.8399999999999997E-3</v>
       </c>
       <c r="J9" s="20">
+        <f t="shared" si="1"/>
+        <v>146.19883040935673</v>
+      </c>
+      <c r="K9" s="20">
         <f t="shared" si="0"/>
-        <v>146.19883040935673</v>
-      </c>
-      <c r="K9" s="20">
-        <f>4/I9</f>
         <v>584.79532163742692</v>
       </c>
       <c r="L9" s="20">
         <v>0.48810799999999999</v>
       </c>
       <c r="M9" s="20">
-        <f t="shared" ref="M9:M13" si="1">L9/$L$7</f>
+        <f t="shared" ref="M9:M13" si="2">L9/$L$7</f>
         <v>2.3479147626148444</v>
       </c>
     </row>
     <row r="10" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="20">
         <v>32</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="21">
         <v>0.37890000000000001</v>
       </c>
@@ -3205,30 +3246,30 @@
         <v>4.8170000000000001E-3</v>
       </c>
       <c r="J10" s="20">
+        <f t="shared" si="1"/>
+        <v>207.59809009757109</v>
+      </c>
+      <c r="K10" s="20">
         <f t="shared" si="0"/>
-        <v>207.59809009757109</v>
-      </c>
-      <c r="K10" s="20">
-        <f>4/I10</f>
         <v>830.39236039028435</v>
       </c>
       <c r="L10" s="20">
         <v>0.41519299999999998</v>
       </c>
       <c r="M10" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9971763913608158</v>
       </c>
     </row>
     <row r="11" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44">
+      <c r="B11" s="45">
         <v>8</v>
       </c>
       <c r="C11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="21">
         <v>0.1166</v>
       </c>
@@ -3242,28 +3283,28 @@
         <v>5.019E-3</v>
       </c>
       <c r="J11" s="20">
+        <f t="shared" si="1"/>
+        <v>199.24287706714486</v>
+      </c>
+      <c r="K11" s="20">
         <f t="shared" si="0"/>
-        <v>199.24287706714486</v>
-      </c>
-      <c r="K11" s="20">
-        <f>4/I11</f>
         <v>796.97150826857944</v>
       </c>
       <c r="L11" s="20">
         <v>0.39848600000000001</v>
       </c>
       <c r="M11" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.916811775458175</v>
       </c>
     </row>
     <row r="12" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="20">
         <v>8</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="21">
         <v>0.2089</v>
       </c>
@@ -3277,28 +3318,28 @@
         <v>4.0899999999999999E-3</v>
       </c>
       <c r="J12" s="20">
+        <f t="shared" si="1"/>
+        <v>244.49877750611248</v>
+      </c>
+      <c r="K12" s="20">
         <f t="shared" si="0"/>
-        <v>244.49877750611248</v>
-      </c>
-      <c r="K12" s="20">
-        <f>4/I12</f>
         <v>977.9951100244499</v>
       </c>
       <c r="L12" s="20">
         <v>0.48898999999999998</v>
       </c>
       <c r="M12" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3521573909278946</v>
       </c>
     </row>
     <row r="13" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="44"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="20">
         <v>16</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="21">
         <v>0.37680000000000002</v>
       </c>
@@ -3312,18 +3353,18 @@
         <v>4.4219999999999997E-3</v>
       </c>
       <c r="J13" s="20">
+        <f t="shared" si="1"/>
+        <v>226.14201718679331</v>
+      </c>
+      <c r="K13" s="20">
         <f t="shared" si="0"/>
-        <v>226.14201718679331</v>
-      </c>
-      <c r="K13" s="20">
-        <f>4/I13</f>
         <v>904.56806874717324</v>
       </c>
       <c r="L13" s="20">
         <v>0.45228299999999999</v>
       </c>
       <c r="M13" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1755880513733223</v>
       </c>
     </row>
@@ -3398,37 +3439,37 @@
       <c r="M18" s="27"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42" t="s">
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
       <c r="M20" s="26"/>
     </row>
     <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -3470,16 +3511,16 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="44">
+      <c r="B22" s="45">
         <v>4</v>
       </c>
       <c r="C22" s="20">
         <v>4</v>
       </c>
-      <c r="D22" s="44">
+      <c r="D22" s="45">
         <v>8192</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="47">
         <v>100</v>
       </c>
       <c r="F22" s="21">
@@ -3509,12 +3550,12 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="20">
         <v>8</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="43"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="21">
         <v>0.11</v>
       </c>
@@ -3537,17 +3578,17 @@
         <v>0.35068199999999999</v>
       </c>
       <c r="M23" s="20">
-        <f t="shared" ref="M23:M28" si="2">L23/$L$22</f>
+        <f t="shared" ref="M23:M28" si="3">L23/$L$22</f>
         <v>0.87138302815554003</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="44"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="20">
         <v>16</v>
       </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="43"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="21">
         <v>0.2036</v>
       </c>
@@ -3570,17 +3611,17 @@
         <v>0.29789300000000002</v>
       </c>
       <c r="M24" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.74021165730302185</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="20">
         <v>32</v>
       </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="43"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="21">
         <v>0.37430000000000002</v>
       </c>
@@ -3603,19 +3644,19 @@
         <v>0.213365</v>
       </c>
       <c r="M25" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.53017445948867292</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="44">
+      <c r="B26" s="45">
         <v>8</v>
       </c>
       <c r="C26" s="20">
         <v>4</v>
       </c>
-      <c r="D26" s="44"/>
-      <c r="E26" s="43"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="21">
         <v>0.11799999999999999</v>
       </c>
@@ -3638,17 +3679,17 @@
         <v>0.358991</v>
       </c>
       <c r="M26" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.89202943025471937</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="44"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="20">
         <v>8</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="43"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="21">
         <v>0.2046</v>
       </c>
@@ -3671,17 +3712,17 @@
         <v>0.29728599999999999</v>
       </c>
       <c r="M27" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.73870336917277724</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="20">
         <v>16</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="43"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="47"/>
       <c r="F28" s="21">
         <v>0.38140000000000002</v>
       </c>
@@ -3704,42 +3745,42 @@
         <v>0.21214</v>
       </c>
       <c r="M28" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.52713055016486809</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="45" t="s">
+      <c r="B43" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42" t="s">
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
       <c r="M44" s="26"/>
     </row>
     <row r="45" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -3781,16 +3822,16 @@
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="44">
+      <c r="B46" s="45">
         <v>4</v>
       </c>
       <c r="C46" s="20">
         <v>4</v>
       </c>
-      <c r="D46" s="44">
+      <c r="D46" s="45">
         <v>8192</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="47">
         <v>200</v>
       </c>
       <c r="F46" s="21">
@@ -3820,12 +3861,12 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
+      <c r="B47" s="45"/>
       <c r="C47" s="20">
         <v>8</v>
       </c>
-      <c r="D47" s="44"/>
-      <c r="E47" s="43"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
@@ -3836,12 +3877,12 @@
       <c r="M47" s="20"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="44"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="20">
         <v>16</v>
       </c>
-      <c r="D48" s="44"/>
-      <c r="E48" s="43"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="47"/>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
@@ -3852,12 +3893,12 @@
       <c r="M48" s="20"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="44"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="20">
         <v>32</v>
       </c>
-      <c r="D49" s="44"/>
-      <c r="E49" s="43"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="47"/>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
       <c r="H49" s="21"/>
@@ -3868,14 +3909,14 @@
       <c r="M49" s="20"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="44">
+      <c r="B50" s="45">
         <v>8</v>
       </c>
       <c r="C50" s="20">
         <v>4</v>
       </c>
-      <c r="D50" s="44"/>
-      <c r="E50" s="43"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="47"/>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
       <c r="H50" s="21"/>
@@ -3886,12 +3927,12 @@
       <c r="M50" s="20"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="44"/>
+      <c r="B51" s="45"/>
       <c r="C51" s="20">
         <v>8</v>
       </c>
-      <c r="D51" s="44"/>
-      <c r="E51" s="43"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="47"/>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
@@ -3902,12 +3943,12 @@
       <c r="M51" s="20"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="44"/>
+      <c r="B52" s="45"/>
       <c r="C52" s="20">
         <v>16</v>
       </c>
-      <c r="D52" s="44"/>
-      <c r="E52" s="43"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="47"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
@@ -3919,11 +3960,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="D7:D13"/>
-    <mergeCell ref="E7:E13"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="E46:E52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B43:M43"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="B19:M19"/>
@@ -3931,18 +3979,11 @@
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:L20"/>
     <mergeCell ref="I5:L5"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B43:M43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="E46:E52"/>
-    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="E7:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3950,6 +3991,580 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:M21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="32"/>
+    </row>
+    <row r="5" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="45">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20">
+        <v>4</v>
+      </c>
+      <c r="D6" s="45">
+        <v>8192</v>
+      </c>
+      <c r="E6" s="47">
+        <v>100</v>
+      </c>
+      <c r="F6" s="21">
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="G6" s="21">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H6" s="21">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="I6" s="20">
+        <v>4.2430000000000002E-3</v>
+      </c>
+      <c r="J6" s="20">
+        <v>14.73</v>
+      </c>
+      <c r="K6" s="20">
+        <v>942.79</v>
+      </c>
+      <c r="L6" s="20">
+        <v>0.47139300000000001</v>
+      </c>
+      <c r="M6" s="20">
+        <f>L6/$L$6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="45"/>
+      <c r="C7" s="20">
+        <v>8</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="21">
+        <v>0.11</v>
+      </c>
+      <c r="G7" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0.15409999999999999</v>
+      </c>
+      <c r="I7" s="20">
+        <v>4.078E-3</v>
+      </c>
+      <c r="J7">
+        <v>7.66</v>
+      </c>
+      <c r="K7" s="20">
+        <v>980.75</v>
+      </c>
+      <c r="L7" s="20">
+        <v>0.49037700000000001</v>
+      </c>
+      <c r="M7" s="20">
+        <f t="shared" ref="M7:M11" si="0">L7/$L$6</f>
+        <v>1.0402721296243262</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="45"/>
+      <c r="C8" s="20">
+        <v>16</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="21">
+        <v>0.2036</v>
+      </c>
+      <c r="G8" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="I8" s="20">
+        <v>4.0080000000000003E-3</v>
+      </c>
+      <c r="J8" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="K8" s="20">
+        <v>998.07</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0.499033</v>
+      </c>
+      <c r="M8" s="20">
+        <f t="shared" si="0"/>
+        <v>1.0586347272869983</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="45">
+        <v>8</v>
+      </c>
+      <c r="C9" s="20">
+        <v>4</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="21">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G9" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0.15790000000000001</v>
+      </c>
+      <c r="I9" s="20">
+        <v>4.176E-3</v>
+      </c>
+      <c r="J9" s="20">
+        <v>7.48</v>
+      </c>
+      <c r="K9" s="20">
+        <v>957.79</v>
+      </c>
+      <c r="L9" s="20">
+        <v>0.47889300000000001</v>
+      </c>
+      <c r="M9" s="20">
+        <f t="shared" si="0"/>
+        <v>1.0159102914128975</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="45"/>
+      <c r="C10" s="20">
+        <v>8</v>
+      </c>
+      <c r="D10" s="45"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="21">
+        <v>0.2046</v>
+      </c>
+      <c r="G10" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="I10" s="20">
+        <v>4.0940000000000004E-3</v>
+      </c>
+      <c r="J10" s="20">
+        <v>3.82</v>
+      </c>
+      <c r="K10" s="20">
+        <v>977.03</v>
+      </c>
+      <c r="L10" s="20">
+        <v>0.48851600000000001</v>
+      </c>
+      <c r="M10" s="20">
+        <f t="shared" si="0"/>
+        <v>1.0363242559817392</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="45"/>
+      <c r="C11" s="20">
+        <v>16</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="21">
+        <v>0.38140000000000002</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0.127</v>
+      </c>
+      <c r="H11" s="21">
+        <v>0.57609999999999995</v>
+      </c>
+      <c r="I11" s="20">
+        <v>3.999E-3</v>
+      </c>
+      <c r="J11" s="20">
+        <v>1.95</v>
+      </c>
+      <c r="K11" s="20">
+        <v>1000.22</v>
+      </c>
+      <c r="L11" s="20">
+        <v>0.500112</v>
+      </c>
+      <c r="M11" s="20">
+        <f t="shared" si="0"/>
+        <v>1.0609236878782671</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="32"/>
+    </row>
+    <row r="15" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="45">
+        <v>4</v>
+      </c>
+      <c r="C16" s="20">
+        <v>4</v>
+      </c>
+      <c r="D16" s="45">
+        <v>8192</v>
+      </c>
+      <c r="E16" s="47">
+        <v>200</v>
+      </c>
+      <c r="F16" s="21">
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H16" s="21">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="I16" s="20">
+        <v>4.2300000000000003E-3</v>
+      </c>
+      <c r="J16" s="20">
+        <v>14.77</v>
+      </c>
+      <c r="K16" s="20">
+        <v>945.58</v>
+      </c>
+      <c r="L16" s="20">
+        <v>0.47279199999999999</v>
+      </c>
+      <c r="M16" s="20">
+        <f>L16/$L$6</f>
+        <v>1.0029677996915525</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="45"/>
+      <c r="C17" s="20">
+        <v>8</v>
+      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="21">
+        <v>0.11</v>
+      </c>
+      <c r="G17" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H17" s="21">
+        <v>0.15409999999999999</v>
+      </c>
+      <c r="I17" s="20">
+        <v>4.0899999999999999E-3</v>
+      </c>
+      <c r="J17">
+        <v>7.64</v>
+      </c>
+      <c r="K17" s="20">
+        <v>977.89</v>
+      </c>
+      <c r="L17" s="20">
+        <v>0.48894300000000002</v>
+      </c>
+      <c r="M17" s="20">
+        <f>L17/$L$6</f>
+        <v>1.0372300819061802</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="45"/>
+      <c r="C18" s="20">
+        <v>16</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="21">
+        <v>0.2036</v>
+      </c>
+      <c r="G18" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H18" s="21">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="I18" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="59"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="45">
+        <v>8</v>
+      </c>
+      <c r="C19" s="20">
+        <v>4</v>
+      </c>
+      <c r="D19" s="45"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="21">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G19" s="21">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="H19" s="21">
+        <v>0.15790000000000001</v>
+      </c>
+      <c r="I19" s="20">
+        <v>4.2570000000000004E-3</v>
+      </c>
+      <c r="J19" s="20">
+        <v>7.34</v>
+      </c>
+      <c r="K19" s="20">
+        <v>939.66</v>
+      </c>
+      <c r="L19" s="20">
+        <v>0.46982800000000002</v>
+      </c>
+      <c r="M19" s="20">
+        <f t="shared" ref="M18:M19" si="1">L19/$L$6</f>
+        <v>0.99668005252517544</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="45"/>
+      <c r="C20" s="20">
+        <v>8</v>
+      </c>
+      <c r="D20" s="45"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="21">
+        <v>0.2046</v>
+      </c>
+      <c r="G20" s="21">
+        <v>6.3500000000000001E-2</v>
+      </c>
+      <c r="H20" s="21">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="I20" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="59"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="45"/>
+      <c r="C21" s="20">
+        <v>16</v>
+      </c>
+      <c r="D21" s="45"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="21">
+        <v>0.38140000000000002</v>
+      </c>
+      <c r="G21" s="21">
+        <v>0.127</v>
+      </c>
+      <c r="H21" s="21">
+        <v>0.57609999999999995</v>
+      </c>
+      <c r="I21" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="D16:D21"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="B9:B11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J12"/>
   <sheetViews>
@@ -3960,16 +4575,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="56"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="23" t="s">
@@ -4001,7 +4616,7 @@
       <c r="C5" s="20">
         <v>8192</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="48">
         <v>8192</v>
       </c>
       <c r="E5" s="20">
@@ -4013,7 +4628,7 @@
       <c r="G5" s="20">
         <v>0.457283</v>
       </c>
-      <c r="H5" s="49">
+      <c r="H5" s="51">
         <v>426.66754193573797</v>
       </c>
       <c r="I5" s="24">
@@ -4028,7 +4643,7 @@
       <c r="C6" s="20">
         <v>16384</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="20">
         <v>134217728</v>
       </c>
@@ -4038,7 +4653,7 @@
       <c r="G6" s="20">
         <v>0.72777099999999995</v>
       </c>
-      <c r="H6" s="50"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="24">
         <v>184.423023</v>
       </c>
@@ -4051,7 +4666,7 @@
       <c r="C7" s="20">
         <v>24576</v>
       </c>
-      <c r="D7" s="47"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="20">
         <v>201326592</v>
       </c>
@@ -4061,7 +4676,7 @@
       <c r="G7" s="20">
         <v>0.99838400000000005</v>
       </c>
-      <c r="H7" s="50"/>
+      <c r="H7" s="52"/>
       <c r="I7" s="24">
         <v>201.65246200000001</v>
       </c>
@@ -4074,7 +4689,7 @@
       <c r="C8" s="20">
         <v>32768</v>
       </c>
-      <c r="D8" s="47"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="20">
         <v>268435456</v>
       </c>
@@ -4084,7 +4699,7 @@
       <c r="G8" s="20">
         <v>1.2690570000000001</v>
       </c>
-      <c r="H8" s="50"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="24">
         <v>211.523561</v>
       </c>
@@ -4097,7 +4712,7 @@
       <c r="C9" s="20">
         <v>40960</v>
       </c>
-      <c r="D9" s="47"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="20">
         <v>335544320</v>
       </c>
@@ -4107,7 +4722,7 @@
       <c r="G9" s="20">
         <v>1.5138590000000001</v>
       </c>
-      <c r="H9" s="50"/>
+      <c r="H9" s="52"/>
       <c r="I9" s="24">
         <v>221.64833100000001</v>
       </c>
@@ -4120,7 +4735,7 @@
       <c r="C10" s="20">
         <v>49152</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="20">
         <v>402653184</v>
       </c>
@@ -4130,7 +4745,7 @@
       <c r="G10" s="20">
         <v>1.756033</v>
       </c>
-      <c r="H10" s="50"/>
+      <c r="H10" s="52"/>
       <c r="I10" s="24">
         <v>229.29704899999999</v>
       </c>
@@ -4143,7 +4758,7 @@
       <c r="C11" s="20">
         <v>57344</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="20">
         <v>469762048</v>
       </c>
@@ -4153,7 +4768,7 @@
       <c r="G11" s="20">
         <v>1.9886269999999999</v>
       </c>
-      <c r="H11" s="50"/>
+      <c r="H11" s="52"/>
       <c r="I11" s="24">
         <v>236.22431399999999</v>
       </c>
@@ -4166,7 +4781,7 @@
       <c r="C12" s="20">
         <v>65536</v>
       </c>
-      <c r="D12" s="48"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="20">
         <v>536870912</v>
       </c>
@@ -4176,7 +4791,7 @@
       <c r="G12" s="20">
         <v>2.1998060000000002</v>
       </c>
-      <c r="H12" s="51"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="24">
         <v>244.053754</v>
       </c>

</xml_diff>

<commit_message>
updated with a plot about trending
</commit_message>
<xml_diff>
--- a/assets/data/SpMV.xlsx
+++ b/assets/data/SpMV.xlsx
@@ -521,6 +521,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,14 +560,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -602,9 +605,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -627,6 +627,599 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>ROM optimization</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1320" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>w/o ROM optimize</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BCSR ROM opt.'!$C$6:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BCSR no ROM opt'!$K$22:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1609.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1402.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1191.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>w/ ROM optimize</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BCSR ROM opt.'!$C$6:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BCSR ROM opt.'!$K$6:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1856.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1872.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2009.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="422264272"/>
+        <c:axId val="427301320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="422264272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>C's</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> value when R=4</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427301320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="427301320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bandwith (MB/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422264272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          <a:cs typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -850,11 +1443,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="430138168"/>
-        <c:axId val="430138560"/>
+        <c:axId val="422260744"/>
+        <c:axId val="422261136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="430138168"/>
+        <c:axId val="422260744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +1555,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430138560"/>
+        <c:crossAx val="422261136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -970,7 +1563,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="430138560"/>
+        <c:axId val="422261136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430138168"/>
+        <c:crossAx val="422260744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1124,6 +1717,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1679,7 +2312,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>484907</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>106628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>173181</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2019,23 +3203,23 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="N2" s="35" t="s">
+      <c r="H2" s="36"/>
+      <c r="N2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
       <c r="T2" s="2"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2086,10 +3270,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="37">
         <v>8192</v>
       </c>
       <c r="C4">
@@ -2110,10 +3294,10 @@
       <c r="H4">
         <v>2.2929999999999999E-3</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="39">
         <v>8192</v>
       </c>
-      <c r="O4" s="36">
+      <c r="O4" s="39">
         <v>1</v>
       </c>
       <c r="P4" s="4">
@@ -2134,8 +3318,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
       <c r="C5">
         <v>2</v>
       </c>
@@ -2154,8 +3338,8 @@
       <c r="H5">
         <v>2.4610000000000001E-3</v>
       </c>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
       <c r="P5" s="4">
         <v>0.1</v>
       </c>
@@ -2174,8 +3358,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="C6">
         <v>4</v>
       </c>
@@ -2194,8 +3378,8 @@
       <c r="H6">
         <v>1.725E-3</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
       <c r="P6" s="4">
         <v>1</v>
       </c>
@@ -2214,8 +3398,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
       <c r="C7">
         <v>8</v>
       </c>
@@ -2234,8 +3418,8 @@
       <c r="H7">
         <v>9.6400000000000001E-4</v>
       </c>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36">
+      <c r="N7" s="39"/>
+      <c r="O7" s="39">
         <v>2</v>
       </c>
       <c r="P7" s="4">
@@ -2256,8 +3440,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
       <c r="P8" s="4">
         <v>0.1</v>
       </c>
@@ -2276,8 +3460,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
       <c r="P9" s="4">
         <v>1</v>
       </c>
@@ -2296,8 +3480,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N10" s="36"/>
-      <c r="O10" s="36">
+      <c r="N10" s="39"/>
+      <c r="O10" s="39">
         <v>4</v>
       </c>
       <c r="P10" s="4">
@@ -2318,8 +3502,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
       <c r="P11" s="4">
         <v>0.1</v>
       </c>
@@ -2338,8 +3522,8 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
       <c r="P12" s="4">
         <v>1</v>
       </c>
@@ -2358,8 +3542,8 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N13" s="36"/>
-      <c r="O13" s="36">
+      <c r="N13" s="39"/>
+      <c r="O13" s="39">
         <v>8</v>
       </c>
       <c r="P13" s="4">
@@ -2380,8 +3564,8 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
       <c r="P14" s="4">
         <v>0.1</v>
       </c>
@@ -2400,8 +3584,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
       <c r="P15" s="4">
         <v>1</v>
       </c>
@@ -2458,72 +3642,72 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="41" t="s">
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="41" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="43"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="46"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="13"/>
       <c r="G4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="2"/>
       <c r="K4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="35"/>
+      <c r="M4" s="38"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="35"/>
+      <c r="Q4" s="38"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
@@ -2574,7 +3758,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="39">
         <v>8192</v>
       </c>
       <c r="B6" s="6">
@@ -2630,7 +3814,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -2687,7 +3871,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="6">
         <v>4</v>
       </c>
@@ -2744,7 +3928,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="6">
         <v>8</v>
       </c>
@@ -2801,7 +3985,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="7">
         <v>16</v>
       </c>
@@ -2858,7 +4042,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="7">
         <v>32</v>
       </c>
@@ -2915,7 +4099,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="7">
         <v>64</v>
       </c>
@@ -2928,24 +4112,24 @@
       <c r="E12" s="8">
         <v>0.54559999999999997</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="39"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="42"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="7">
         <v>128</v>
       </c>
@@ -2973,7 +4157,7 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="7">
         <v>256</v>
       </c>
@@ -3030,8 +4214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:M52"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3048,37 +4232,37 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
     </row>
     <row r="5" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
       <c r="M5" s="26"/>
     </row>
     <row r="6" spans="2:13" s="18" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3120,16 +4304,16 @@
       </c>
     </row>
     <row r="7" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46">
+      <c r="B7" s="50">
         <v>4</v>
       </c>
       <c r="C7" s="20">
         <v>4</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="50">
         <v>8192</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="50">
         <v>100</v>
       </c>
       <c r="F7" s="21">
@@ -3149,8 +4333,8 @@
         <v>103.95010395010395</v>
       </c>
       <c r="K7" s="20">
-        <f t="shared" ref="K7:K13" si="0">4/I7</f>
-        <v>415.80041580041581</v>
+        <f>4/I7*2</f>
+        <v>831.60083160083161</v>
       </c>
       <c r="L7" s="20">
         <v>0.20788999999999999</v>
@@ -3161,12 +4345,12 @@
       </c>
     </row>
     <row r="8" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
       <c r="F8" s="21">
         <v>0.1137</v>
       </c>
@@ -3180,12 +4364,12 @@
         <v>5.0090000000000004E-3</v>
       </c>
       <c r="J8" s="20">
-        <f t="shared" ref="J8:J13" si="1">1/I8</f>
+        <f t="shared" ref="J8:J13" si="0">1/I8</f>
         <v>199.64064683569572</v>
       </c>
       <c r="K8" s="20">
-        <f t="shared" si="0"/>
-        <v>798.56258734278288</v>
+        <f t="shared" ref="K8:K13" si="1">4/I8*2</f>
+        <v>1597.1251746855658</v>
       </c>
       <c r="L8" s="20">
         <v>0.39931</v>
@@ -3196,12 +4380,12 @@
       </c>
     </row>
     <row r="9" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="20">
         <v>16</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="21">
         <v>0.20280000000000001</v>
       </c>
@@ -3215,12 +4399,12 @@
         <v>6.8399999999999997E-3</v>
       </c>
       <c r="J9" s="20">
+        <f t="shared" si="0"/>
+        <v>146.19883040935673</v>
+      </c>
+      <c r="K9" s="20">
         <f t="shared" si="1"/>
-        <v>146.19883040935673</v>
-      </c>
-      <c r="K9" s="20">
-        <f t="shared" si="0"/>
-        <v>584.79532163742692</v>
+        <v>1169.5906432748538</v>
       </c>
       <c r="L9" s="20">
         <v>0.48810799999999999</v>
@@ -3231,12 +4415,12 @@
       </c>
     </row>
     <row r="10" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="20">
         <v>32</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="21">
         <v>0.37890000000000001</v>
       </c>
@@ -3250,12 +4434,12 @@
         <v>4.8170000000000001E-3</v>
       </c>
       <c r="J10" s="20">
+        <f t="shared" si="0"/>
+        <v>207.59809009757109</v>
+      </c>
+      <c r="K10" s="20">
         <f t="shared" si="1"/>
-        <v>207.59809009757109</v>
-      </c>
-      <c r="K10" s="20">
-        <f t="shared" si="0"/>
-        <v>830.39236039028435</v>
+        <v>1660.7847207805687</v>
       </c>
       <c r="L10" s="20">
         <v>0.41519299999999998</v>
@@ -3266,14 +4450,14 @@
       </c>
     </row>
     <row r="11" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46">
+      <c r="B11" s="50">
         <v>8</v>
       </c>
       <c r="C11" s="20">
         <v>4</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="21">
         <v>0.1166</v>
       </c>
@@ -3287,12 +4471,12 @@
         <v>5.019E-3</v>
       </c>
       <c r="J11" s="20">
+        <f t="shared" si="0"/>
+        <v>199.24287706714486</v>
+      </c>
+      <c r="K11" s="20">
         <f t="shared" si="1"/>
-        <v>199.24287706714486</v>
-      </c>
-      <c r="K11" s="20">
-        <f t="shared" si="0"/>
-        <v>796.97150826857944</v>
+        <v>1593.9430165371589</v>
       </c>
       <c r="L11" s="20">
         <v>0.39848600000000001</v>
@@ -3303,12 +4487,12 @@
       </c>
     </row>
     <row r="12" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="20">
         <v>8</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="21">
         <v>0.2089</v>
       </c>
@@ -3322,12 +4506,12 @@
         <v>4.0899999999999999E-3</v>
       </c>
       <c r="J12" s="20">
+        <f t="shared" si="0"/>
+        <v>244.49877750611248</v>
+      </c>
+      <c r="K12" s="20">
         <f t="shared" si="1"/>
-        <v>244.49877750611248</v>
-      </c>
-      <c r="K12" s="20">
-        <f t="shared" si="0"/>
-        <v>977.9951100244499</v>
+        <v>1955.9902200488998</v>
       </c>
       <c r="L12" s="20">
         <v>0.48898999999999998</v>
@@ -3338,12 +4522,12 @@
       </c>
     </row>
     <row r="13" spans="2:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="46"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="20">
         <v>16</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="21">
         <v>0.37680000000000002</v>
       </c>
@@ -3357,12 +4541,12 @@
         <v>4.4219999999999997E-3</v>
       </c>
       <c r="J13" s="20">
+        <f t="shared" si="0"/>
+        <v>226.14201718679331</v>
+      </c>
+      <c r="K13" s="20">
         <f t="shared" si="1"/>
-        <v>226.14201718679331</v>
-      </c>
-      <c r="K13" s="20">
-        <f t="shared" si="0"/>
-        <v>904.56806874717324</v>
+        <v>1809.1361374943465</v>
       </c>
       <c r="L13" s="20">
         <v>0.45228299999999999</v>
@@ -3443,37 +4627,37 @@
       <c r="M18" s="27"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44" t="s">
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
       <c r="M20" s="26"/>
     </row>
     <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -3515,16 +4699,16 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="46">
+      <c r="B22" s="50">
         <v>4</v>
       </c>
       <c r="C22" s="20">
         <v>4</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D22" s="50">
         <v>8192</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="49">
         <v>100</v>
       </c>
       <c r="F22" s="21">
@@ -3543,7 +4727,8 @@
         <v>12.58</v>
       </c>
       <c r="K22" s="20">
-        <v>804.89</v>
+        <f>804.89*2</f>
+        <v>1609.78</v>
       </c>
       <c r="L22" s="20">
         <v>0.402443</v>
@@ -3554,12 +4739,12 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="20">
         <v>8</v>
       </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="45"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="21">
         <v>0.11</v>
       </c>
@@ -3576,7 +4761,8 @@
         <v>5.48</v>
       </c>
       <c r="K23" s="20">
-        <v>701.36</v>
+        <f>701.36*2</f>
+        <v>1402.72</v>
       </c>
       <c r="L23" s="20">
         <v>0.35068199999999999</v>
@@ -3587,12 +4773,12 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="20">
         <v>16</v>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="45"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="21">
         <v>0.2036</v>
       </c>
@@ -3609,7 +4795,8 @@
         <v>2.33</v>
       </c>
       <c r="K24" s="20">
-        <v>595.79</v>
+        <f>595.79*2</f>
+        <v>1191.58</v>
       </c>
       <c r="L24" s="20">
         <v>0.29789300000000002</v>
@@ -3620,12 +4807,12 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="46"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="20">
         <v>32</v>
       </c>
-      <c r="D25" s="46"/>
-      <c r="E25" s="45"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="21">
         <v>0.37430000000000002</v>
       </c>
@@ -3642,7 +4829,8 @@
         <v>0.83</v>
       </c>
       <c r="K25" s="20">
-        <v>426.73</v>
+        <f>426.73*2</f>
+        <v>853.46</v>
       </c>
       <c r="L25" s="20">
         <v>0.213365</v>
@@ -3653,14 +4841,14 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="46">
+      <c r="B26" s="50">
         <v>8</v>
       </c>
       <c r="C26" s="20">
         <v>4</v>
       </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="45"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="21">
         <v>0.11799999999999999</v>
       </c>
@@ -3677,7 +4865,8 @@
         <v>5.61</v>
       </c>
       <c r="K26" s="20">
-        <v>717.98</v>
+        <f>717.98*2</f>
+        <v>1435.96</v>
       </c>
       <c r="L26" s="20">
         <v>0.358991</v>
@@ -3688,12 +4877,12 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="46"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="20">
         <v>8</v>
       </c>
-      <c r="D27" s="46"/>
-      <c r="E27" s="45"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="21">
         <v>0.2046</v>
       </c>
@@ -3710,7 +4899,8 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="K27" s="20">
-        <v>594.57000000000005</v>
+        <f>594.57*2</f>
+        <v>1189.1400000000001</v>
       </c>
       <c r="L27" s="20">
         <v>0.29728599999999999</v>
@@ -3721,12 +4911,12 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="46"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="20">
         <v>16</v>
       </c>
-      <c r="D28" s="46"/>
-      <c r="E28" s="45"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="21">
         <v>0.38140000000000002</v>
       </c>
@@ -3743,7 +4933,8 @@
         <v>0.83</v>
       </c>
       <c r="K28" s="20">
-        <v>424.28</v>
+        <f>424.28*2</f>
+        <v>848.56</v>
       </c>
       <c r="L28" s="20">
         <v>0.21214</v>
@@ -3754,37 +4945,37 @@
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="47"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44" t="s">
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
       <c r="M44" s="26"/>
     </row>
     <row r="45" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -3826,16 +5017,16 @@
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="46">
+      <c r="B46" s="50">
         <v>4</v>
       </c>
       <c r="C46" s="20">
         <v>4</v>
       </c>
-      <c r="D46" s="46">
+      <c r="D46" s="50">
         <v>8192</v>
       </c>
-      <c r="E46" s="45">
+      <c r="E46" s="49">
         <v>200</v>
       </c>
       <c r="F46" s="21">
@@ -3854,7 +5045,8 @@
         <v>239.4</v>
       </c>
       <c r="K46" s="20">
-        <v>957.62</v>
+        <f>957.62*2</f>
+        <v>1915.24</v>
       </c>
       <c r="L46" s="20">
         <v>0.47880800000000001</v>
@@ -3865,12 +5057,12 @@
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="46"/>
+      <c r="B47" s="50"/>
       <c r="C47" s="20">
         <v>8</v>
       </c>
-      <c r="D47" s="46"/>
-      <c r="E47" s="45"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="49"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
@@ -3881,12 +5073,12 @@
       <c r="M47" s="20"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="46"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="20">
         <v>16</v>
       </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="45"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="49"/>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
@@ -3897,12 +5089,12 @@
       <c r="M48" s="20"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="46"/>
+      <c r="B49" s="50"/>
       <c r="C49" s="20">
         <v>32</v>
       </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="45"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="49"/>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
       <c r="H49" s="21"/>
@@ -3913,14 +5105,14 @@
       <c r="M49" s="20"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="46">
+      <c r="B50" s="50">
         <v>8</v>
       </c>
       <c r="C50" s="20">
         <v>4</v>
       </c>
-      <c r="D50" s="46"/>
-      <c r="E50" s="45"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="49"/>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
       <c r="H50" s="21"/>
@@ -3931,12 +5123,12 @@
       <c r="M50" s="20"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="46"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="20">
         <v>8</v>
       </c>
-      <c r="D51" s="46"/>
-      <c r="E51" s="45"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="49"/>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
@@ -3947,12 +5139,12 @@
       <c r="M51" s="20"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="46"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="20">
         <v>16</v>
       </c>
-      <c r="D52" s="46"/>
-      <c r="E52" s="45"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="49"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
@@ -3964,6 +5156,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="E46:E52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B43:M43"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="B19:M19"/>
@@ -3976,18 +5180,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="D7:D13"/>
     <mergeCell ref="E7:E13"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B43:M43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="E46:E52"/>
-    <mergeCell ref="B50:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3999,7 +5191,7 @@
   <dimension ref="B3:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4015,37 +5207,37 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="32"/>
     </row>
     <row r="5" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -4087,16 +5279,16 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="46">
+      <c r="B6" s="50">
         <v>4</v>
       </c>
       <c r="C6" s="20">
         <v>4</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="50">
         <v>8192</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="49">
         <v>100</v>
       </c>
       <c r="F6" s="21">
@@ -4108,30 +5300,30 @@
       <c r="H6" s="21">
         <v>8.4599999999999995E-2</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="33">
         <v>4.444E-3</v>
       </c>
-      <c r="J6" s="61">
+      <c r="J6" s="34">
         <v>14.06</v>
       </c>
       <c r="K6" s="20">
         <v>1856.24</v>
       </c>
-      <c r="L6" s="60">
+      <c r="L6" s="33">
         <v>0.44999800000000001</v>
       </c>
-      <c r="M6" s="61">
+      <c r="M6" s="34">
         <f>L6/$L$6</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="46"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="20">
         <v>8</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="45"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="49"/>
       <c r="F7" s="21">
         <v>0.11</v>
       </c>
@@ -4141,30 +5333,30 @@
       <c r="H7" s="21">
         <v>0.15409999999999999</v>
       </c>
-      <c r="I7" s="60">
+      <c r="I7" s="33">
         <v>4.339E-3</v>
       </c>
-      <c r="J7" s="62">
+      <c r="J7" s="35">
         <v>7.2</v>
       </c>
       <c r="K7" s="20">
         <v>1872.69</v>
       </c>
-      <c r="L7" s="60">
+      <c r="L7" s="33">
         <v>0.46097100000000002</v>
       </c>
-      <c r="M7" s="61">
+      <c r="M7" s="34">
         <f t="shared" ref="M7:M11" si="0">L7/$L$6</f>
         <v>1.0243845528202349</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="20">
         <v>16</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="45"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="21">
         <v>0.2036</v>
       </c>
@@ -4174,32 +5366,32 @@
       <c r="H8" s="21">
         <v>0.29320000000000002</v>
       </c>
-      <c r="I8" s="60">
+      <c r="I8" s="33">
         <v>4.0119999999999999E-3</v>
       </c>
-      <c r="J8" s="61">
+      <c r="J8" s="34">
         <v>3.89</v>
       </c>
       <c r="K8" s="20">
         <v>2009.54</v>
       </c>
-      <c r="L8" s="60">
+      <c r="L8" s="33">
         <v>0.49848999999999999</v>
       </c>
-      <c r="M8" s="61">
+      <c r="M8" s="34">
         <f t="shared" si="0"/>
         <v>1.1077604789354618</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="46">
+      <c r="B9" s="50">
         <v>8</v>
       </c>
       <c r="C9" s="20">
         <v>4</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="45"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="21">
         <v>0.11799999999999999</v>
       </c>
@@ -4209,30 +5401,30 @@
       <c r="H9" s="21">
         <v>0.15790000000000001</v>
       </c>
-      <c r="I9" s="60">
+      <c r="I9" s="33">
         <v>4.3579999999999999E-3</v>
       </c>
-      <c r="J9" s="61">
+      <c r="J9" s="34">
         <v>7.17</v>
       </c>
       <c r="K9" s="20">
         <v>1864.23</v>
       </c>
-      <c r="L9" s="60">
+      <c r="L9" s="33">
         <v>0.45888800000000002</v>
       </c>
-      <c r="M9" s="61">
+      <c r="M9" s="34">
         <f t="shared" si="0"/>
         <v>1.019755643358415</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="20">
         <v>8</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="45"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="21">
         <v>0.2046</v>
       </c>
@@ -4242,30 +5434,30 @@
       <c r="H10" s="21">
         <v>0.29699999999999999</v>
       </c>
-      <c r="I10" s="60">
+      <c r="I10" s="33">
         <v>4.3E-3</v>
       </c>
-      <c r="J10" s="61">
+      <c r="J10" s="34">
         <v>3.63</v>
       </c>
       <c r="K10" s="20">
         <v>1875.17</v>
       </c>
-      <c r="L10" s="60">
+      <c r="L10" s="33">
         <v>0.46515899999999999</v>
       </c>
-      <c r="M10" s="61">
+      <c r="M10" s="34">
         <f t="shared" si="0"/>
         <v>1.0336912608500481</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="20">
         <v>16</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="45"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="21">
         <v>0.38140000000000002</v>
       </c>
@@ -4275,55 +5467,55 @@
       <c r="H11" s="21">
         <v>0.57609999999999995</v>
       </c>
-      <c r="I11" s="60">
+      <c r="I11" s="33">
         <v>4.2170000000000003E-3</v>
       </c>
-      <c r="J11" s="61">
+      <c r="J11" s="34">
         <v>1.85</v>
       </c>
       <c r="K11" s="20">
         <v>1904.48</v>
       </c>
-      <c r="L11" s="60">
+      <c r="L11" s="33">
         <v>0.47426699999999999</v>
       </c>
-      <c r="M11" s="61">
+      <c r="M11" s="34">
         <f t="shared" si="0"/>
         <v>1.0539313508060035</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44" t="s">
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
       <c r="M14" s="32"/>
     </row>
     <row r="15" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -4365,16 +5557,16 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="46">
+      <c r="B16" s="50">
         <v>4</v>
       </c>
       <c r="C16" s="20">
         <v>4</v>
       </c>
-      <c r="D16" s="46">
+      <c r="D16" s="50">
         <v>8192</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="49">
         <v>200</v>
       </c>
       <c r="F16" s="21">
@@ -4404,12 +5596,12 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="20">
         <v>8</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="45"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="21">
         <v>0.11</v>
       </c>
@@ -4437,12 +5629,12 @@
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="20">
         <v>16</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="45"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="21">
         <v>0.2036</v>
       </c>
@@ -4452,23 +5644,23 @@
       <c r="H18" s="21">
         <v>0.29320000000000002</v>
       </c>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="50"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="53"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="46">
+      <c r="B19" s="50">
         <v>8</v>
       </c>
       <c r="C19" s="20">
         <v>4</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="45"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="49"/>
       <c r="F19" s="21">
         <v>0.11799999999999999</v>
       </c>
@@ -4496,12 +5688,12 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="20">
         <v>8</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="45"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="49"/>
       <c r="F20" s="21">
         <v>0.2046</v>
       </c>
@@ -4511,21 +5703,21 @@
       <c r="H20" s="21">
         <v>0.29699999999999999</v>
       </c>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="50"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="53"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="20">
         <v>16</v>
       </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="49"/>
       <c r="F21" s="21">
         <v>0.38140000000000002</v>
       </c>
@@ -4535,24 +5727,16 @@
       <c r="H21" s="21">
         <v>0.57609999999999995</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="50"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="E6:E11"/>
-    <mergeCell ref="B9:B11"/>
     <mergeCell ref="I18:M18"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="B14:E14"/>
@@ -4564,9 +5748,18 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="I20:M20"/>
     <mergeCell ref="I21:M21"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4581,16 +5774,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="59"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="23" t="s">
@@ -4622,7 +5815,7 @@
       <c r="C5" s="20">
         <v>8192</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="54">
         <v>8192</v>
       </c>
       <c r="E5" s="20">
@@ -4634,7 +5827,7 @@
       <c r="G5" s="20">
         <v>0.457283</v>
       </c>
-      <c r="H5" s="54">
+      <c r="H5" s="57">
         <v>426.66754193573797</v>
       </c>
       <c r="I5" s="24">
@@ -4649,7 +5842,7 @@
       <c r="C6" s="20">
         <v>16384</v>
       </c>
-      <c r="D6" s="52"/>
+      <c r="D6" s="55"/>
       <c r="E6" s="20">
         <v>134217728</v>
       </c>
@@ -4659,7 +5852,7 @@
       <c r="G6" s="20">
         <v>0.72777099999999995</v>
       </c>
-      <c r="H6" s="55"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="24">
         <v>184.423023</v>
       </c>
@@ -4672,7 +5865,7 @@
       <c r="C7" s="20">
         <v>24576</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="20">
         <v>201326592</v>
       </c>
@@ -4682,7 +5875,7 @@
       <c r="G7" s="20">
         <v>0.99838400000000005</v>
       </c>
-      <c r="H7" s="55"/>
+      <c r="H7" s="58"/>
       <c r="I7" s="24">
         <v>201.65246200000001</v>
       </c>
@@ -4695,7 +5888,7 @@
       <c r="C8" s="20">
         <v>32768</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="20">
         <v>268435456</v>
       </c>
@@ -4705,7 +5898,7 @@
       <c r="G8" s="20">
         <v>1.2690570000000001</v>
       </c>
-      <c r="H8" s="55"/>
+      <c r="H8" s="58"/>
       <c r="I8" s="24">
         <v>211.523561</v>
       </c>
@@ -4718,7 +5911,7 @@
       <c r="C9" s="20">
         <v>40960</v>
       </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="55"/>
       <c r="E9" s="20">
         <v>335544320</v>
       </c>
@@ -4728,7 +5921,7 @@
       <c r="G9" s="20">
         <v>1.5138590000000001</v>
       </c>
-      <c r="H9" s="55"/>
+      <c r="H9" s="58"/>
       <c r="I9" s="24">
         <v>221.64833100000001</v>
       </c>
@@ -4741,7 +5934,7 @@
       <c r="C10" s="20">
         <v>49152</v>
       </c>
-      <c r="D10" s="52"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="20">
         <v>402653184</v>
       </c>
@@ -4751,7 +5944,7 @@
       <c r="G10" s="20">
         <v>1.756033</v>
       </c>
-      <c r="H10" s="55"/>
+      <c r="H10" s="58"/>
       <c r="I10" s="24">
         <v>229.29704899999999</v>
       </c>
@@ -4764,7 +5957,7 @@
       <c r="C11" s="20">
         <v>57344</v>
       </c>
-      <c r="D11" s="52"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="20">
         <v>469762048</v>
       </c>
@@ -4774,7 +5967,7 @@
       <c r="G11" s="20">
         <v>1.9886269999999999</v>
       </c>
-      <c r="H11" s="55"/>
+      <c r="H11" s="58"/>
       <c r="I11" s="24">
         <v>236.22431399999999</v>
       </c>
@@ -4787,7 +5980,7 @@
       <c r="C12" s="20">
         <v>65536</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="20">
         <v>536870912</v>
       </c>
@@ -4797,7 +5990,7 @@
       <c r="G12" s="20">
         <v>2.1998060000000002</v>
       </c>
-      <c r="H12" s="56"/>
+      <c r="H12" s="59"/>
       <c r="I12" s="24">
         <v>244.053754</v>
       </c>

</xml_diff>